<commit_message>
property descriptors added to excel file, absolute value of volume and correct formula for eccentricity added.
</commit_message>
<xml_diff>
--- a/filter.xlsx
+++ b/filter.xlsx
@@ -547,10 +547,10 @@
         <v>0.4960846663548496</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.00969472079893333</v>
+        <v>0.00969472079893333</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2323938204721279</v>
+        <v>11.48535503315988</v>
       </c>
       <c r="M2" t="n">
         <v>1.000334897085503</v>
@@ -607,7 +607,7 @@
         <v>0.01590439131051608</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3427123403481196</v>
+        <v>7.099637412920116</v>
       </c>
       <c r="M3" t="n">
         <v>1.040871367211538</v>
@@ -661,10 +661,10 @@
         <v>0.543397952857855</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.01325426013973928</v>
+        <v>0.01325426013973928</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3062020031952402</v>
+        <v>8.075894559567743</v>
       </c>
       <c r="M4" t="n">
         <v>1.000087842446218</v>
@@ -718,10 +718,10 @@
         <v>0.6841060218526565</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.01639692088266616</v>
+        <v>0.01639692088266616</v>
       </c>
       <c r="L5" t="n">
-        <v>0.5600793972448161</v>
+        <v>10.52914882324945</v>
       </c>
       <c r="M5" t="n">
         <v>1.019602982013704</v>
@@ -775,10 +775,10 @@
         <v>0.6257623516403885</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.01306959244847502</v>
+        <v>0.01306959244847502</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4158825699016632</v>
+        <v>12.68387135099335</v>
       </c>
       <c r="M6" t="n">
         <v>1.000015334816036</v>
@@ -835,7 +835,7 @@
         <v>0.01295409530763829</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7844989522342387</v>
+        <v>22.94731378212609</v>
       </c>
       <c r="M7" t="n">
         <v>1.017566755312438</v>
@@ -892,7 +892,7 @@
         <v>0.01908562329087091</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8844322507555199</v>
+        <v>12.44549290361185</v>
       </c>
       <c r="M8" t="n">
         <v>1.030677872462861</v>
@@ -949,7 +949,7 @@
         <v>0.009975970967985805</v>
       </c>
       <c r="L9" t="n">
-        <v>0.2600306686388594</v>
+        <v>15.07908937091644</v>
       </c>
       <c r="M9" t="n">
         <v>1.005869176797269</v>
@@ -1006,7 +1006,7 @@
         <v>0.01255561436367198</v>
       </c>
       <c r="L10" t="n">
-        <v>0.444660889065681</v>
+        <v>13.59841524742389</v>
       </c>
       <c r="M10" t="n">
         <v>1.000101082498449</v>
@@ -1060,10 +1060,10 @@
         <v>0.5155323991472338</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.007621731315349026</v>
+        <v>0.007621731315349026</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2596832313546892</v>
+        <v>20.85490661336506</v>
       </c>
       <c r="M11" t="n">
         <v>1.002407120968962</v>
@@ -1120,7 +1120,7 @@
         <v>0.01123623370532281</v>
       </c>
       <c r="L12" t="n">
-        <v>0.3286656920541874</v>
+        <v>12.06550250529592</v>
       </c>
       <c r="M12" t="n">
         <v>1.000098181321785</v>
@@ -1177,7 +1177,7 @@
         <v>0.008542724197583795</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2255609091304601</v>
+        <v>14.31549912731494</v>
       </c>
       <c r="M13" t="n">
         <v>1.000124583200261</v>
@@ -1234,7 +1234,7 @@
         <v>0.008688156177072196</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2070726049691317</v>
+        <v>13.18528179680904</v>
       </c>
       <c r="M14" t="n">
         <v>1.000262014827568</v>
@@ -1291,7 +1291,7 @@
         <v>0.009759242445778932</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2142974789387195</v>
+        <v>10.42377814679937</v>
       </c>
       <c r="M15" t="n">
         <v>1.000034862569707</v>
@@ -1348,7 +1348,7 @@
         <v>0.01835451586876079</v>
       </c>
       <c r="L16" t="n">
-        <v>1.077288421633996</v>
+        <v>15.79502363977216</v>
       </c>
       <c r="M16" t="n">
         <v>1.002880364900019</v>
@@ -1402,10 +1402,10 @@
         <v>0.5999072416381481</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.01491488341990384</v>
+        <v>0.01491488341990384</v>
       </c>
       <c r="L17" t="n">
-        <v>0.377948953649073</v>
+        <v>8.581440856746253</v>
       </c>
       <c r="M17" t="n">
         <v>1.015178790335268</v>
@@ -1459,10 +1459,10 @@
         <v>0.6531055878851733</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01406293312406702</v>
+        <v>0.01406293312406702</v>
       </c>
       <c r="L18" t="n">
-        <v>0.460919847837964</v>
+        <v>12.45506510980057</v>
       </c>
       <c r="M18" t="n">
         <v>1.02177406652802</v>
@@ -1516,10 +1516,10 @@
         <v>0.7360984179166513</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.01465912640700348</v>
+        <v>0.01465912640700348</v>
       </c>
       <c r="L19" t="n">
-        <v>0.6365599574596588</v>
+        <v>16.41115320549832</v>
       </c>
       <c r="M19" t="n">
         <v>1.05254524203714</v>
@@ -1573,10 +1573,10 @@
         <v>0.7853326990300168</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.01576448600290746</v>
+        <v>0.01576448600290746</v>
       </c>
       <c r="L20" t="n">
-        <v>0.6673571979487208</v>
+        <v>17.23252978851101</v>
       </c>
       <c r="M20" t="n">
         <v>1.114969126568778</v>
@@ -1630,10 +1630,10 @@
         <v>0.7850400121457435</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.01568640550832293</v>
+        <v>0.01568640550832293</v>
       </c>
       <c r="L21" t="n">
-        <v>0.754569353456843</v>
+        <v>17.38505739203211</v>
       </c>
       <c r="M21" t="n">
         <v>1.065873754703805</v>
@@ -1687,10 +1687,10 @@
         <v>0.9119319935651532</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.02173702527560601</v>
+        <v>0.02173702527560601</v>
       </c>
       <c r="L22" t="n">
-        <v>1.118320032652237</v>
+        <v>14.19171114869982</v>
       </c>
       <c r="M22" t="n">
         <v>1.070937685467958</v>
@@ -1747,7 +1747,7 @@
         <v>0.01609747321899925</v>
       </c>
       <c r="L23" t="n">
-        <v>0.5272000012215033</v>
+        <v>10.26043949404444</v>
       </c>
       <c r="M23" t="n">
         <v>1.020128502600102</v>
@@ -1804,7 +1804,7 @@
         <v>0.0274509333944279</v>
       </c>
       <c r="L24" t="n">
-        <v>1.242577999277773</v>
+        <v>9.95091492844425</v>
       </c>
       <c r="M24" t="n">
         <v>1.079138861842041</v>
@@ -1858,10 +1858,10 @@
         <v>0.7060022366776144</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.01798698143372966</v>
+        <v>0.01798698143372966</v>
       </c>
       <c r="L25" t="n">
-        <v>0.5678874823639325</v>
+        <v>9.617214102401558</v>
       </c>
       <c r="M25" t="n">
         <v>1.051644275822808</v>
@@ -1915,10 +1915,10 @@
         <v>0.8922048674293137</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.02301508962428604</v>
+        <v>0.02301508962428604</v>
       </c>
       <c r="L26" t="n">
-        <v>0.8576265437203334</v>
+        <v>11.85539559587097</v>
       </c>
       <c r="M26" t="n">
         <v>1.138695029883829</v>
@@ -1972,10 +1972,10 @@
         <v>0.825477115790038</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.02116753214885932</v>
+        <v>0.02116753214885932</v>
       </c>
       <c r="L27" t="n">
-        <v>0.8933099985105007</v>
+        <v>11.09998225979092</v>
       </c>
       <c r="M27" t="n">
         <v>1.050627703117698</v>
@@ -2029,10 +2029,10 @@
         <v>0.7869410565744875</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.02240344211934422</v>
+        <v>0.02240344211934422</v>
       </c>
       <c r="L28" t="n">
-        <v>0.7589577792160828</v>
+        <v>8.585087773166201</v>
       </c>
       <c r="M28" t="n">
         <v>1.060947225825897</v>
@@ -2086,10 +2086,10 @@
         <v>0.8306116626916157</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.02434886894471254</v>
+        <v>0.02434886894471254</v>
       </c>
       <c r="L29" t="n">
-        <v>0.8458449345630774</v>
+        <v>8.546417734925132</v>
       </c>
       <c r="M29" t="n">
         <v>1.065417693066996</v>
@@ -2143,10 +2143,10 @@
         <v>0.8666745031907841</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.02353756616712649</v>
+        <v>0.02353756616712649</v>
       </c>
       <c r="L30" t="n">
-        <v>1.08920864520885</v>
+        <v>10.389450525882</v>
       </c>
       <c r="M30" t="n">
         <v>1.027014653566677</v>
@@ -2200,10 +2200,10 @@
         <v>0.8163909905542953</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01849064569187966</v>
+        <v>0.01849064569187966</v>
       </c>
       <c r="L31" t="n">
-        <v>0.9009665677198335</v>
+        <v>14.07142507639476</v>
       </c>
       <c r="M31" t="n">
         <v>1.04172312592171</v>
@@ -2257,10 +2257,10 @@
         <v>0.8298002336743958</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.02173129578325216</v>
+        <v>0.02173129578325216</v>
       </c>
       <c r="L32" t="n">
-        <v>0.9713687010928737</v>
+        <v>10.69786317323081</v>
       </c>
       <c r="M32" t="n">
         <v>1.018764876983673</v>
@@ -2317,7 +2317,7 @@
         <v>0.02607198537606692</v>
       </c>
       <c r="L33" t="n">
-        <v>1.209601618705232</v>
+        <v>9.783587280511284</v>
       </c>
       <c r="M33" t="n">
         <v>1.025717396182617</v>
@@ -2371,10 +2371,10 @@
         <v>0.620371439467041</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.01535130082482646</v>
+        <v>0.01535130082482646</v>
       </c>
       <c r="L34" t="n">
-        <v>0.3860772605302198</v>
+        <v>8.958032814714551</v>
       </c>
       <c r="M34" t="n">
         <v>1.036274963347565</v>
@@ -2428,10 +2428,10 @@
         <v>0.9029345760093276</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.02742890278182571</v>
+        <v>0.02742890278182571</v>
       </c>
       <c r="L35" t="n">
-        <v>1.090664430438818</v>
+        <v>8.651663258372841</v>
       </c>
       <c r="M35" t="n">
         <v>1.067527178718424</v>
@@ -2488,7 +2488,7 @@
         <v>0.02051707285402443</v>
       </c>
       <c r="L36" t="n">
-        <v>0.8677048560578169</v>
+        <v>14.71477910244634</v>
       </c>
       <c r="M36" t="n">
         <v>1.14179467688772</v>
@@ -2545,7 +2545,7 @@
         <v>0.01888417060564004</v>
       </c>
       <c r="L37" t="n">
-        <v>0.6440637659370837</v>
+        <v>8.763817379401527</v>
       </c>
       <c r="M37" t="n">
         <v>1.011590370690777</v>
@@ -2599,10 +2599,10 @@
         <v>1.0366373074294</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.02622607252667206</v>
+        <v>0.02622607252667206</v>
       </c>
       <c r="L38" t="n">
-        <v>1.260611736294827</v>
+        <v>14.32061319495503</v>
       </c>
       <c r="M38" t="n">
         <v>1.185816739579525</v>
@@ -2656,10 +2656,10 @@
         <v>0.8023640680326584</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.01807966741699047</v>
+        <v>0.01807966741699047</v>
       </c>
       <c r="L39" t="n">
-        <v>0.853621938612677</v>
+        <v>13.97272677831034</v>
       </c>
       <c r="M39" t="n">
         <v>1.042778690150219</v>
@@ -2713,10 +2713,10 @@
         <v>0.7384847421315958</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.02105510646938236</v>
+        <v>0.02105510646938236</v>
       </c>
       <c r="L40" t="n">
-        <v>0.5837301369432984</v>
+        <v>8.032621865681193</v>
       </c>
       <c r="M40" t="n">
         <v>1.092024850647776</v>
@@ -2770,10 +2770,10 @@
         <v>0.9158378501330964</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.02170113782560266</v>
+        <v>0.02170113782560266</v>
       </c>
       <c r="L41" t="n">
-        <v>0.8945505206128154</v>
+        <v>14.42242804629338</v>
       </c>
       <c r="M41" t="n">
         <v>1.164879736894012</v>
@@ -2830,7 +2830,7 @@
         <v>0.07090444908801205</v>
       </c>
       <c r="L42" t="n">
-        <v>4.016147299730244</v>
+        <v>7.634523428688026</v>
       </c>
       <c r="M42" t="n">
         <v>1.255834143554525</v>
@@ -2884,10 +2884,10 @@
         <v>1.36934246148538</v>
       </c>
       <c r="K43" t="n">
-        <v>-0.05391250773975407</v>
+        <v>0.05391250773975407</v>
       </c>
       <c r="L43" t="n">
-        <v>2.991811805758136</v>
+        <v>7.810966682043879</v>
       </c>
       <c r="M43" t="n">
         <v>1.177445584411009</v>
@@ -2941,10 +2941,10 @@
         <v>0.9650482150613996</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.0300595919726747</v>
+        <v>0.0300595919726747</v>
       </c>
       <c r="L44" t="n">
-        <v>0.9580305355786142</v>
+        <v>8.794851271115949</v>
       </c>
       <c r="M44" t="n">
         <v>1.209917474132584</v>
@@ -3001,7 +3001,7 @@
         <v>0.06100233802040718</v>
       </c>
       <c r="L45" t="n">
-        <v>4.494796910164519</v>
+        <v>7.520650369747928</v>
       </c>
       <c r="M45" t="n">
         <v>1.087987850703398</v>
@@ -3055,10 +3055,10 @@
         <v>1.53030210634383</v>
       </c>
       <c r="K46" t="n">
-        <v>-0.06318460608148606</v>
+        <v>0.06318460608148606</v>
       </c>
       <c r="L46" t="n">
-        <v>4.853215962028768</v>
+        <v>7.937003833736317</v>
       </c>
       <c r="M46" t="n">
         <v>1.092965345361747</v>
@@ -3115,7 +3115,7 @@
         <v>0.0712223439452245</v>
       </c>
       <c r="L47" t="n">
-        <v>8.578124719524853</v>
+        <v>8.839777566261038</v>
       </c>
       <c r="M47" t="n">
         <v>1.041304518823451</v>
@@ -3169,10 +3169,10 @@
         <v>1.681599146932731</v>
       </c>
       <c r="K48" t="n">
-        <v>-0.07007114626238599</v>
+        <v>0.07007114626238599</v>
       </c>
       <c r="L48" t="n">
-        <v>5.573880227523526</v>
+        <v>8.563210455586612</v>
       </c>
       <c r="M48" t="n">
         <v>1.167272878630291</v>
@@ -3226,10 +3226,10 @@
         <v>1.665212591495297</v>
       </c>
       <c r="K49" t="n">
-        <v>-0.07103163381718668</v>
+        <v>0.07103163381718668</v>
       </c>
       <c r="L49" t="n">
-        <v>6.391403586618891</v>
+        <v>8.091947878511585</v>
       </c>
       <c r="M49" t="n">
         <v>1.081640888106733</v>
@@ -3286,7 +3286,7 @@
         <v>0.03744830926195438</v>
       </c>
       <c r="L50" t="n">
-        <v>1.987242190139608</v>
+        <v>8.562732608081072</v>
       </c>
       <c r="M50" t="n">
         <v>1.015865229395025</v>
@@ -3343,7 +3343,7 @@
         <v>0.03910664130091772</v>
       </c>
       <c r="L51" t="n">
-        <v>1.58060834931266</v>
+        <v>9.895510914995871</v>
       </c>
       <c r="M51" t="n">
         <v>1.258772105625239</v>
@@ -3397,10 +3397,10 @@
         <v>1.111755210206269</v>
       </c>
       <c r="K52" t="n">
-        <v>-0.04048045713548196</v>
+        <v>0.04048045713548196</v>
       </c>
       <c r="L52" t="n">
-        <v>2.598191967356596</v>
+        <v>7.414542013015462</v>
       </c>
       <c r="M52" t="n">
         <v>1.002946016342454</v>
@@ -3457,7 +3457,7 @@
         <v>0.0644499281945512</v>
       </c>
       <c r="L53" t="n">
-        <v>3.645694070252942</v>
+        <v>6.886303738557961</v>
       </c>
       <c r="M53" t="n">
         <v>1.15791181233156</v>
@@ -3511,10 +3511,10 @@
         <v>1.3939563703379</v>
       </c>
       <c r="K54" t="n">
-        <v>-0.0593172599228336</v>
+        <v>0.0593172599228336</v>
       </c>
       <c r="L54" t="n">
-        <v>2.828667089237045</v>
+        <v>6.806643531552895</v>
       </c>
       <c r="M54" t="n">
         <v>1.221542881525743</v>
@@ -3568,10 +3568,10 @@
         <v>0.8827426365601513</v>
       </c>
       <c r="K55" t="n">
-        <v>-0.02805898243395404</v>
+        <v>0.02805898243395404</v>
       </c>
       <c r="L55" t="n">
-        <v>0.7432520887598196</v>
+        <v>7.725135448662849</v>
       </c>
       <c r="M55" t="n">
         <v>1.204449711693894</v>
@@ -3628,7 +3628,7 @@
         <v>0.05014641305060946</v>
       </c>
       <c r="L56" t="n">
-        <v>2.487823345572501</v>
+        <v>5.507364150040838</v>
       </c>
       <c r="M56" t="n">
         <v>1.06009321302585</v>
@@ -3682,10 +3682,10 @@
         <v>1.368844508422907</v>
       </c>
       <c r="K57" t="n">
-        <v>-0.06030320602414591</v>
+        <v>0.06030320602414591</v>
       </c>
       <c r="L57" t="n">
-        <v>3.40767197508073</v>
+        <v>6.236331267469521</v>
       </c>
       <c r="M57" t="n">
         <v>1.099952788470356</v>
@@ -3739,10 +3739,10 @@
         <v>1.79506287657195</v>
       </c>
       <c r="K58" t="n">
-        <v>-0.08791164930650511</v>
+        <v>0.08791164930650511</v>
       </c>
       <c r="L58" t="n">
-        <v>7.248062824639983</v>
+        <v>6.617497212208145</v>
       </c>
       <c r="M58" t="n">
         <v>1.150482559319484</v>
@@ -3799,7 +3799,7 @@
         <v>0.07651286124020035</v>
       </c>
       <c r="L59" t="n">
-        <v>5.151499302769569</v>
+        <v>7.369896837253499</v>
       </c>
       <c r="M59" t="n">
         <v>1.209741520987533</v>
@@ -3853,10 +3853,10 @@
         <v>1.636034282261475</v>
       </c>
       <c r="K60" t="n">
-        <v>-0.07381795785875644</v>
+        <v>0.07381795785875644</v>
       </c>
       <c r="L60" t="n">
-        <v>5.595942381076398</v>
+        <v>7.105600283637971</v>
       </c>
       <c r="M60" t="n">
         <v>1.109617078212908</v>
@@ -3913,7 +3913,7 @@
         <v>0.0374937379461246</v>
       </c>
       <c r="L61" t="n">
-        <v>1.711209147285342</v>
+        <v>7.491567941747965</v>
       </c>
       <c r="M61" t="n">
         <v>1.022091591440362</v>
@@ -3970,7 +3970,7 @@
         <v>0.03228122052951639</v>
       </c>
       <c r="L62" t="n">
-        <v>0.7764134942531804</v>
+        <v>3.645257612449891</v>
       </c>
       <c r="M62" t="n">
         <v>1.013917625466348</v>
@@ -4027,7 +4027,7 @@
         <v>0.0322811522413278</v>
       </c>
       <c r="L63" t="n">
-        <v>0.7764131326205336</v>
+        <v>3.645263364308688</v>
       </c>
       <c r="M63" t="n">
         <v>1.013917112779471</v>
@@ -4084,7 +4084,7 @@
         <v>0.03231725012797861</v>
       </c>
       <c r="L64" t="n">
-        <v>0.7772813257116943</v>
+        <v>3.645263197409369</v>
       </c>
       <c r="M64" t="n">
         <v>1.014294922869684</v>
@@ -4138,10 +4138,10 @@
         <v>1.305640094582188</v>
       </c>
       <c r="K65" t="n">
-        <v>-0.08823569887563076</v>
+        <v>0.08823569887563076</v>
       </c>
       <c r="L65" t="n">
-        <v>3.56628427655868</v>
+        <v>2.527722542392933</v>
       </c>
       <c r="M65" t="n">
         <v>1.059306823344003</v>
@@ -4195,10 +4195,10 @@
         <v>1.302081890742085</v>
       </c>
       <c r="K66" t="n">
-        <v>-0.08672960346322278</v>
+        <v>0.08672960346322278</v>
       </c>
       <c r="L66" t="n">
-        <v>3.580396194509249</v>
+        <v>2.594942873278541</v>
       </c>
       <c r="M66" t="n">
         <v>1.055113294247733</v>
@@ -4252,10 +4252,10 @@
         <v>1.304598060992846</v>
       </c>
       <c r="K67" t="n">
-        <v>-0.087461869744175</v>
+        <v>0.087461869744175</v>
       </c>
       <c r="L67" t="n">
-        <v>3.586482496390853</v>
+        <v>2.566494263504979</v>
       </c>
       <c r="M67" t="n">
         <v>1.05657743869636</v>
@@ -4312,7 +4312,7 @@
         <v>0.09702355557990375</v>
       </c>
       <c r="L68" t="n">
-        <v>3.419645955939809</v>
+        <v>1.952324417428741</v>
       </c>
       <c r="M68" t="n">
         <v>1.050914015811669</v>
@@ -4369,7 +4369,7 @@
         <v>0.01578883407185881</v>
       </c>
       <c r="L69" t="n">
-        <v>0.20341589963528</v>
+        <v>3.83950629043699</v>
       </c>
       <c r="M69" t="n">
         <v>1.005091133296479</v>
@@ -4423,10 +4423,10 @@
         <v>0.4764437856085031</v>
       </c>
       <c r="K70" t="n">
-        <v>-0.01578169317574656</v>
+        <v>0.01578169317574656</v>
       </c>
       <c r="L70" t="n">
-        <v>0.2033233048745891</v>
+        <v>3.839506748697421</v>
       </c>
       <c r="M70" t="n">
         <v>1.004940637857597</v>
@@ -4483,7 +4483,7 @@
         <v>0.01573364332131156</v>
       </c>
       <c r="L71" t="n">
-        <v>0.1983255326935414</v>
+        <v>3.76469966274482</v>
       </c>
       <c r="M71" t="n">
         <v>1.004612604616788</v>
@@ -4537,10 +4537,10 @@
         <v>0.7742418133324078</v>
       </c>
       <c r="K72" t="n">
-        <v>-0.03669269994136076</v>
+        <v>0.03669269994136076</v>
       </c>
       <c r="L72" t="n">
-        <v>0.8234605900107181</v>
+        <v>3.048022393937595</v>
       </c>
       <c r="M72" t="n">
         <v>1.022157016562245</v>
@@ -4594,10 +4594,10 @@
         <v>0.7815419750000263</v>
       </c>
       <c r="K73" t="n">
-        <v>-0.03811733831031597</v>
+        <v>0.03811733831031597</v>
       </c>
       <c r="L73" t="n">
-        <v>0.8474299132909201</v>
+        <v>2.905088834354112</v>
       </c>
       <c r="M73" t="n">
         <v>1.022184584007483</v>
@@ -4651,10 +4651,10 @@
         <v>0.4210693298019003</v>
       </c>
       <c r="K74" t="n">
-        <v>-0.01186401469429861</v>
+        <v>0.01186401469429861</v>
       </c>
       <c r="L74" t="n">
-        <v>0.1413360337372732</v>
+        <v>4.689700433128499</v>
       </c>
       <c r="M74" t="n">
         <v>1.002793504860442</v>
@@ -4711,7 +4711,7 @@
         <v>0.02404743505357006</v>
       </c>
       <c r="L75" t="n">
-        <v>0.4107828381785034</v>
+        <v>3.536926972384843</v>
       </c>
       <c r="M75" t="n">
         <v>1.022431829501334</v>
@@ -4765,10 +4765,10 @@
         <v>0.4097177967330162</v>
       </c>
       <c r="K76" t="n">
-        <v>-0.01207350307936912</v>
+        <v>0.01207350307936912</v>
       </c>
       <c r="L76" t="n">
-        <v>0.1294337210953213</v>
+        <v>4.171915639713506</v>
       </c>
       <c r="M76" t="n">
         <v>1.004930765640634</v>
@@ -4822,10 +4822,10 @@
         <v>0.4096828644733591</v>
       </c>
       <c r="K77" t="n">
-        <v>-0.01207354320079256</v>
+        <v>0.01207354320079256</v>
       </c>
       <c r="L77" t="n">
-        <v>0.1294003082372086</v>
+        <v>4.170820926519117</v>
       </c>
       <c r="M77" t="n">
         <v>1.004931566550158</v>
@@ -4879,10 +4879,10 @@
         <v>0.4659217491788874</v>
       </c>
       <c r="K78" t="n">
-        <v>-0.007473378907255569</v>
+        <v>0.007473378907255569</v>
       </c>
       <c r="L78" t="n">
-        <v>0.1867235292735789</v>
+        <v>16.01225780619437</v>
       </c>
       <c r="M78" t="n">
         <v>1.011378601047651</v>
@@ -4939,7 +4939,7 @@
         <v>0.05454584709005973</v>
       </c>
       <c r="L79" t="n">
-        <v>5.219377633973201</v>
+        <v>11.82420346850279</v>
       </c>
       <c r="M79" t="n">
         <v>1.075710825565384</v>
@@ -4996,7 +4996,7 @@
         <v>0.05436424613796407</v>
       </c>
       <c r="L80" t="n">
-        <v>5.203111477900135</v>
+        <v>11.82674680728329</v>
       </c>
       <c r="M80" t="n">
         <v>1.074521325503073</v>
@@ -5050,10 +5050,10 @@
         <v>0.6539364161162503</v>
       </c>
       <c r="K81" t="n">
-        <v>-0.02598740739480469</v>
+        <v>0.02598740739480469</v>
       </c>
       <c r="L81" t="n">
-        <v>0.5111453874470018</v>
+        <v>3.661240733756365</v>
       </c>
       <c r="M81" t="n">
         <v>1.014402741836897</v>
@@ -5107,10 +5107,10 @@
         <v>0.3522015986765618</v>
       </c>
       <c r="K82" t="n">
-        <v>-0.006759236397633026</v>
+        <v>0.006759236397633026</v>
       </c>
       <c r="L82" t="n">
-        <v>0.08189314508638938</v>
+        <v>8.455247484646078</v>
       </c>
       <c r="M82" t="n">
         <v>1.000015504778809</v>
@@ -5167,7 +5167,7 @@
         <v>0.02372873034442956</v>
       </c>
       <c r="L83" t="n">
-        <v>1.157928680851469</v>
+        <v>9.873059104571908</v>
       </c>
       <c r="M83" t="n">
         <v>1.000042751727084</v>
@@ -5221,10 +5221,10 @@
         <v>0.3503236000555149</v>
       </c>
       <c r="K84" t="n">
-        <v>-0.007137663178552878</v>
+        <v>0.007137663178552878</v>
       </c>
       <c r="L84" t="n">
-        <v>0.08197537844984643</v>
+        <v>7.461801848747795</v>
       </c>
       <c r="M84" t="n">
         <v>1.000024956105038</v>
@@ -5281,7 +5281,7 @@
         <v>0.007810890887763962</v>
       </c>
       <c r="L85" t="n">
-        <v>0.1713629853201263</v>
+        <v>13.19393613773101</v>
       </c>
       <c r="M85" t="n">
         <v>1.000487460385972</v>
@@ -5335,10 +5335,10 @@
         <v>0.735911658741736</v>
       </c>
       <c r="K86" t="n">
-        <v>-0.01490794501726879</v>
+        <v>0.01490794501726879</v>
       </c>
       <c r="L86" t="n">
-        <v>0.7360927957823042</v>
+        <v>15.85583478293001</v>
       </c>
       <c r="M86" t="n">
         <v>1.000066005245711</v>
@@ -5392,10 +5392,10 @@
         <v>0.4293202085323519</v>
       </c>
       <c r="K87" t="n">
-        <v>-0.007916365156034309</v>
+        <v>0.007916365156034309</v>
       </c>
       <c r="L87" t="n">
-        <v>0.1508168552588827</v>
+        <v>11.16451815549995</v>
       </c>
       <c r="M87" t="n">
         <v>1.000028035899353</v>
@@ -5452,7 +5452,7 @@
         <v>0.01217868445952127</v>
       </c>
       <c r="L88" t="n">
-        <v>0.4171907912751263</v>
+        <v>13.03305341041775</v>
       </c>
       <c r="M88" t="n">
         <v>1.000116539356065</v>
@@ -5506,10 +5506,10 @@
         <v>1.564762460066097</v>
       </c>
       <c r="K89" t="n">
-        <v>-0.04240800020180689</v>
+        <v>0.04240800020180689</v>
       </c>
       <c r="L89" t="n">
-        <v>3.391932709997191</v>
+        <v>18.83637359106723</v>
       </c>
       <c r="M89" t="n">
         <v>1.181230477322599</v>
@@ -5566,7 +5566,7 @@
         <v>0.005949277342073391</v>
       </c>
       <c r="L90" t="n">
-        <v>0.08814294373611449</v>
+        <v>11.65076057514636</v>
       </c>
       <c r="M90" t="n">
         <v>1.002490384034293</v>
@@ -5620,10 +5620,10 @@
         <v>0.4619074853412483</v>
       </c>
       <c r="K91" t="n">
-        <v>-0.007798521195669306</v>
+        <v>0.007798521195669306</v>
       </c>
       <c r="L91" t="n">
-        <v>0.1215000674967863</v>
+        <v>14.32808381417829</v>
       </c>
       <c r="M91" t="n">
         <v>1.000487618110749</v>
@@ -5677,10 +5677,10 @@
         <v>0.3503236000555149</v>
       </c>
       <c r="K92" t="n">
-        <v>-0.007137663178552878</v>
+        <v>0.007137663178552878</v>
       </c>
       <c r="L92" t="n">
-        <v>0.08197537844984643</v>
+        <v>7.461801848747795</v>
       </c>
       <c r="M92" t="n">
         <v>1.000024956105038</v>
@@ -5737,7 +5737,7 @@
         <v>0.01620146373133698</v>
       </c>
       <c r="L93" t="n">
-        <v>0.6981633779463906</v>
+        <v>13.27365054926682</v>
       </c>
       <c r="M93" t="n">
         <v>1.000000942550649</v>
@@ -5791,10 +5791,10 @@
         <v>0.6637214387582092</v>
       </c>
       <c r="K94" t="n">
-        <v>-0.01311622289208005</v>
+        <v>0.01311622289208005</v>
       </c>
       <c r="L94" t="n">
-        <v>0.5132160300702039</v>
+        <v>15.02752945128997</v>
       </c>
       <c r="M94" t="n">
         <v>1.002734612548859</v>
@@ -5848,10 +5848,10 @@
         <v>0.3810114221400956</v>
       </c>
       <c r="K95" t="n">
-        <v>-0.006014567430845618</v>
+        <v>0.006014567430845618</v>
       </c>
       <c r="L95" t="n">
-        <v>0.09053353898493394</v>
+        <v>13.51925675440159</v>
       </c>
       <c r="M95" t="n">
         <v>1.000000950009998</v>
@@ -5905,10 +5905,10 @@
         <v>0.5284772430488514</v>
       </c>
       <c r="K96" t="n">
-        <v>-0.01198865165524572</v>
+        <v>0.01198865165524572</v>
       </c>
       <c r="L96" t="n">
-        <v>0.2511218126926499</v>
+        <v>9.079999317533884</v>
       </c>
       <c r="M96" t="n">
         <v>1.000010289243029</v>
@@ -5965,7 +5965,7 @@
         <v>0.01619686791930201</v>
       </c>
       <c r="L97" t="n">
-        <v>0.2562615921375128</v>
+        <v>10.16695862645441</v>
       </c>
       <c r="M97" t="n">
         <v>1.116270991484307</v>
@@ -6019,10 +6019,10 @@
         <v>0.5293984764410083</v>
       </c>
       <c r="K98" t="n">
-        <v>-0.004745131071005795</v>
+        <v>0.004745131071005795</v>
       </c>
       <c r="L98" t="n">
-        <v>0.1944490079814192</v>
+        <v>58.26386110835634</v>
       </c>
       <c r="M98" t="n">
         <v>1.001667957621565</v>
@@ -6079,7 +6079,7 @@
         <v>0.02879938992530991</v>
       </c>
       <c r="L99" t="n">
-        <v>2.584400643412658</v>
+        <v>22.00603152538715</v>
       </c>
       <c r="M99" t="n">
         <v>1.047821242557548</v>
@@ -6136,7 +6136,7 @@
         <v>0.02571551895775465</v>
       </c>
       <c r="L100" t="n">
-        <v>1.531514293996074</v>
+        <v>11.08752266861298</v>
       </c>
       <c r="M100" t="n">
         <v>1.00075025303026</v>
@@ -6193,7 +6193,7 @@
         <v>0.04043881218646748</v>
       </c>
       <c r="L101" t="n">
-        <v>3.503148977292054</v>
+        <v>14.8674216695726</v>
       </c>
       <c r="M101" t="n">
         <v>1.029794666125545</v>
@@ -6247,10 +6247,10 @@
         <v>1.359558923131599</v>
       </c>
       <c r="K102" t="n">
-        <v>-0.08987985052701755</v>
+        <v>0.08987985052701755</v>
       </c>
       <c r="L102" t="n">
-        <v>4.37715072144131</v>
+        <v>2.750534187561975</v>
       </c>
       <c r="M102" t="n">
         <v>1.028996712382677</v>
@@ -6307,7 +6307,7 @@
         <v>0.1336771465750493</v>
       </c>
       <c r="L103" t="n">
-        <v>11.63453378675662</v>
+        <v>3.512868813199104</v>
       </c>
       <c r="M103" t="n">
         <v>1.0445202290029</v>
@@ -6364,7 +6364,7 @@
         <v>0.1667967527571254</v>
       </c>
       <c r="L104" t="n">
-        <v>10.53897171586234</v>
+        <v>3.029686495471644</v>
       </c>
       <c r="M104" t="n">
         <v>1.196132881565648</v>
@@ -6418,10 +6418,10 @@
         <v>1.192293093582505</v>
       </c>
       <c r="K105" t="n">
-        <v>-0.06147716080338628</v>
+        <v>0.06147716080338628</v>
       </c>
       <c r="L105" t="n">
-        <v>3.070703098940194</v>
+        <v>3.965236606092163</v>
       </c>
       <c r="M105" t="n">
         <v>1.009805292814719</v>
@@ -6475,10 +6475,10 @@
         <v>2.512051378039318</v>
       </c>
       <c r="K106" t="n">
-        <v>-0.1992360322569151</v>
+        <v>0.1992360322569151</v>
       </c>
       <c r="L106" t="n">
-        <v>20.59920835531777</v>
+        <v>3.530997506383666</v>
       </c>
       <c r="M106" t="n">
         <v>1.133735757933138</v>
@@ -6535,7 +6535,7 @@
         <v>0.1231927098767763</v>
       </c>
       <c r="L107" t="n">
-        <v>7.17064910208605</v>
+        <v>2.399615193316545</v>
       </c>
       <c r="M107" t="n">
         <v>1.002005827186056</v>
@@ -6592,7 +6592,7 @@
         <v>0.2539782108981502</v>
       </c>
       <c r="L108" t="n">
-        <v>22.10016326365959</v>
+        <v>2.229545106017587</v>
       </c>
       <c r="M108" t="n">
         <v>1.113606208300756</v>
@@ -6646,10 +6646,10 @@
         <v>2.414623371193488</v>
       </c>
       <c r="K109" t="n">
-        <v>-0.2700506493203574</v>
+        <v>0.2700506493203574</v>
       </c>
       <c r="L109" t="n">
-        <v>23.61781636525567</v>
+        <v>1.706889372642604</v>
       </c>
       <c r="M109" t="n">
         <v>1.024380264370306</v>
@@ -6706,7 +6706,7 @@
         <v>0.1567521931290388</v>
       </c>
       <c r="L110" t="n">
-        <v>13.64377141633233</v>
+        <v>2.585810788725782</v>
       </c>
       <c r="M110" t="n">
         <v>1.001014471238148</v>
@@ -6760,10 +6760,10 @@
         <v>2.245663351560956</v>
       </c>
       <c r="K111" t="n">
-        <v>-0.2614261214773336</v>
+        <v>0.2614261214773336</v>
       </c>
       <c r="L111" t="n">
-        <v>19.5614476289401</v>
+        <v>1.465155168961974</v>
       </c>
       <c r="M111" t="n">
         <v>1.002124470404045</v>
@@ -6817,10 +6817,10 @@
         <v>1.844105022765052</v>
       </c>
       <c r="K112" t="n">
-        <v>-0.1258550789516125</v>
+        <v>0.1258550789516125</v>
       </c>
       <c r="L112" t="n">
-        <v>10.87054141956303</v>
+        <v>3.500766027772983</v>
       </c>
       <c r="M112" t="n">
         <v>1.016045263775337</v>
@@ -6874,10 +6874,10 @@
         <v>2.242435973919155</v>
       </c>
       <c r="K113" t="n">
-        <v>-0.1695366431851443</v>
+        <v>0.1695366431851443</v>
       </c>
       <c r="L113" t="n">
-        <v>14.14003411919548</v>
+        <v>3.468810878059028</v>
       </c>
       <c r="M113" t="n">
         <v>1.056134378159364</v>
@@ -6934,7 +6934,7 @@
         <v>0.158026806657007</v>
       </c>
       <c r="L114" t="n">
-        <v>16.03643468656177</v>
+        <v>3.335918239689899</v>
       </c>
       <c r="M114" t="n">
         <v>1.01304108802372</v>
@@ -6991,7 +6991,7 @@
         <v>0.1347230536912881</v>
       </c>
       <c r="L115" t="n">
-        <v>7.181526857124332</v>
+        <v>3.250665878882905</v>
       </c>
       <c r="M115" t="n">
         <v>1.12913256452641</v>
@@ -7048,7 +7048,7 @@
         <v>0.2604694862523141</v>
       </c>
       <c r="L116" t="n">
-        <v>17.6538401032094</v>
+        <v>1.88625271703691</v>
       </c>
       <c r="M116" t="n">
         <v>1.160955160373396</v>
@@ -7102,10 +7102,10 @@
         <v>2.293394951557198</v>
       </c>
       <c r="K117" t="n">
-        <v>-0.2037402892868402</v>
+        <v>0.2037402892868402</v>
       </c>
       <c r="L117" t="n">
-        <v>16.84830762278348</v>
+        <v>2.569391872846627</v>
       </c>
       <c r="M117" t="n">
         <v>1.109043439954926</v>
@@ -7159,10 +7159,10 @@
         <v>1.727232380811006</v>
       </c>
       <c r="K118" t="n">
-        <v>-0.1623926613559631</v>
+        <v>0.1623926613559631</v>
       </c>
       <c r="L118" t="n">
-        <v>9.691146745800776</v>
+        <v>1.727695259696937</v>
       </c>
       <c r="M118" t="n">
         <v>1.004515556487618</v>
@@ -7216,10 +7216,10 @@
         <v>1.906627166011909</v>
       </c>
       <c r="K119" t="n">
-        <v>-0.1550878733957261</v>
+        <v>0.1550878733957261</v>
       </c>
       <c r="L119" t="n">
-        <v>8.623653403464232</v>
+        <v>2.547940457178622</v>
       </c>
       <c r="M119" t="n">
         <v>1.150483045234404</v>
@@ -7273,10 +7273,10 @@
         <v>1.681665020542338</v>
       </c>
       <c r="K120" t="n">
-        <v>-0.151092348866972</v>
+        <v>0.151092348866972</v>
       </c>
       <c r="L120" t="n">
-        <v>8.69587694547039</v>
+        <v>1.841964064940788</v>
       </c>
       <c r="M120" t="n">
         <v>1.010905205881191</v>
@@ -7333,7 +7333,7 @@
         <v>0.2433853101742524</v>
       </c>
       <c r="L121" t="n">
-        <v>20.48279784992331</v>
+        <v>2.356704250830725</v>
       </c>
       <c r="M121" t="n">
         <v>1.050652006721155</v>
@@ -7387,10 +7387,10 @@
         <v>0.6860613658971985</v>
       </c>
       <c r="K122" t="n">
-        <v>-0.009439567285755904</v>
+        <v>0.009439567285755904</v>
       </c>
       <c r="L122" t="n">
-        <v>0.5180521766310066</v>
+        <v>32.04293910639947</v>
       </c>
       <c r="M122" t="n">
         <v>1.059257719490895</v>
@@ -7447,7 +7447,7 @@
         <v>0.02152319511939498</v>
       </c>
       <c r="L123" t="n">
-        <v>2.328039104432567</v>
+        <v>28.31749393392657</v>
       </c>
       <c r="M123" t="n">
         <v>1.066962910709601</v>
@@ -7501,10 +7501,10 @@
         <v>0.7975610374943033</v>
       </c>
       <c r="K124" t="n">
-        <v>-0.01471960970881142</v>
+        <v>0.01471960970881142</v>
       </c>
       <c r="L124" t="n">
-        <v>0.7971768401078644</v>
+        <v>20.70364564391438</v>
       </c>
       <c r="M124" t="n">
         <v>1.064924766418411</v>
@@ -7561,7 +7561,7 @@
         <v>0.0121554686443321</v>
       </c>
       <c r="L125" t="n">
-        <v>0.8637537343256656</v>
+        <v>42.03731551086255</v>
       </c>
       <c r="M125" t="n">
         <v>1.158100697722159</v>
@@ -7618,7 +7618,7 @@
         <v>0.0127364451882323</v>
       </c>
       <c r="L126" t="n">
-        <v>1.030271948605149</v>
+        <v>46.08308914129115</v>
       </c>
       <c r="M126" t="n">
         <v>1.161570400542528</v>
@@ -7675,7 +7675,7 @@
         <v>0.02267595003325515</v>
       </c>
       <c r="L127" t="n">
-        <v>2.700988109471834</v>
+        <v>34.10608242698109</v>
       </c>
       <c r="M127" t="n">
         <v>1.118316598050626</v>
@@ -7729,10 +7729,10 @@
         <v>1.11376945626094</v>
       </c>
       <c r="K128" t="n">
-        <v>-0.0212488742797054</v>
+        <v>0.0212488742797054</v>
       </c>
       <c r="L128" t="n">
-        <v>2.170910297584747</v>
+        <v>27.0558812271612</v>
       </c>
       <c r="M128" t="n">
         <v>1.067140928636082</v>
@@ -7789,7 +7789,7 @@
         <v>0.01840335684291367</v>
       </c>
       <c r="L129" t="n">
-        <v>1.708831531587485</v>
+        <v>25.73278056536103</v>
       </c>
       <c r="M129" t="n">
         <v>1.032655558515852</v>
@@ -7846,7 +7846,7 @@
         <v>0.01626612991272035</v>
       </c>
       <c r="L130" t="n">
-        <v>0.7103528405349631</v>
+        <v>19.60901095089019</v>
       </c>
       <c r="M130" t="n">
         <v>1.16312578475269</v>
@@ -7900,10 +7900,10 @@
         <v>1.063697748091409</v>
       </c>
       <c r="K131" t="n">
-        <v>-0.01778698526245418</v>
+        <v>0.01778698526245418</v>
       </c>
       <c r="L131" t="n">
-        <v>0.9940325262275187</v>
+        <v>33.63548199879326</v>
       </c>
       <c r="M131" t="n">
         <v>1.321992953187229</v>
@@ -7957,10 +7957,10 @@
         <v>1.018234724879014</v>
       </c>
       <c r="K132" t="n">
-        <v>-0.01733038460164736</v>
+        <v>0.01733038460164736</v>
       </c>
       <c r="L132" t="n">
-        <v>0.8741146214356403</v>
+        <v>31.0795653122637</v>
       </c>
       <c r="M132" t="n">
         <v>1.321103885025926</v>
@@ -8014,10 +8014,10 @@
         <v>0.9924076700546227</v>
       </c>
       <c r="K133" t="n">
-        <v>-0.01864903593297213</v>
+        <v>0.01864903593297213</v>
       </c>
       <c r="L133" t="n">
-        <v>1.371645329183009</v>
+        <v>24.84878689262071</v>
       </c>
       <c r="M133" t="n">
         <v>1.108075523765166</v>
@@ -8071,10 +8071,10 @@
         <v>0.8551511151299622</v>
       </c>
       <c r="K134" t="n">
-        <v>-0.01282149059912036</v>
+        <v>0.01282149059912036</v>
       </c>
       <c r="L134" t="n">
-        <v>1.058868166158131</v>
+        <v>33.63560077651999</v>
       </c>
       <c r="M134" t="n">
         <v>1.040154827201399</v>
@@ -8128,10 +8128,10 @@
         <v>0.5650373974379259</v>
       </c>
       <c r="K135" t="n">
-        <v>-0.008905861084369464</v>
+        <v>0.008905861084369464</v>
       </c>
       <c r="L135" t="n">
-        <v>0.1832131695635407</v>
+        <v>20.1107085415053</v>
       </c>
       <c r="M135" t="n">
         <v>1.234024349072804</v>
@@ -8185,10 +8185,10 @@
         <v>0.7918253691215809</v>
       </c>
       <c r="K136" t="n">
-        <v>-0.01189365515676166</v>
+        <v>0.01189365515676166</v>
       </c>
       <c r="L136" t="n">
-        <v>0.8419196556078987</v>
+        <v>31.03167208150994</v>
       </c>
       <c r="M136" t="n">
         <v>1.039896182485802</v>
@@ -8245,7 +8245,7 @@
         <v>0.02702739659579552</v>
       </c>
       <c r="L137" t="n">
-        <v>2.973616234016975</v>
+        <v>31.44598507791763</v>
       </c>
       <c r="M137" t="n">
         <v>1.176101995131973</v>
@@ -8302,7 +8302,7 @@
         <v>0.02368007370948014</v>
       </c>
       <c r="L138" t="n">
-        <v>4.115857286170456</v>
+        <v>70.59365683778263</v>
       </c>
       <c r="M138" t="n">
         <v>1.275365210226366</v>
@@ -8359,7 +8359,7 @@
         <v>0.01118651182527476</v>
       </c>
       <c r="L139" t="n">
-        <v>0.5412791068651256</v>
+        <v>24.94362978184407</v>
       </c>
       <c r="M139" t="n">
         <v>1.073998204470807</v>
@@ -8413,10 +8413,10 @@
         <v>1.412240379811059</v>
       </c>
       <c r="K140" t="n">
-        <v>-0.02829743948302985</v>
+        <v>0.02829743948302985</v>
       </c>
       <c r="L140" t="n">
-        <v>2.463062600879863</v>
+        <v>31.10134866047153</v>
       </c>
       <c r="M140" t="n">
         <v>1.295947315651011</v>
@@ -8470,10 +8470,10 @@
         <v>1.000234841321089</v>
       </c>
       <c r="K141" t="n">
-        <v>-0.01688736787277194</v>
+        <v>0.01688736787277194</v>
       </c>
       <c r="L141" t="n">
-        <v>1.396273022126033</v>
+        <v>31.02627469574041</v>
       </c>
       <c r="M141" t="n">
         <v>1.107328628466576</v>
@@ -8530,7 +8530,7 @@
         <v>0.08068342425333851</v>
       </c>
       <c r="L142" t="n">
-        <v>46.24665388517197</v>
+        <v>38.75948597261728</v>
       </c>
       <c r="M142" t="n">
         <v>1.023562045235944</v>
@@ -8587,7 +8587,7 @@
         <v>0.138471557629765</v>
       </c>
       <c r="L143" t="n">
-        <v>75.14360379002311</v>
+        <v>22.26980230793001</v>
       </c>
       <c r="M143" t="n">
         <v>1.06860520007195</v>
@@ -8641,10 +8641,10 @@
         <v>2.661254058597339</v>
       </c>
       <c r="K144" t="n">
-        <v>-0.08146385468848881</v>
+        <v>0.08146385468848881</v>
       </c>
       <c r="L144" t="n">
-        <v>34.15021101199502</v>
+        <v>25.11173529014368</v>
       </c>
       <c r="M144" t="n">
         <v>1.016099274131933</v>
@@ -8698,10 +8698,10 @@
         <v>3.620383357285565</v>
       </c>
       <c r="K145" t="n">
-        <v>-0.170242756213572</v>
+        <v>0.170242756213572</v>
       </c>
       <c r="L145" t="n">
-        <v>73.72942849430966</v>
+        <v>14.47684825597645</v>
       </c>
       <c r="M145" t="n">
         <v>1.068465232425221</v>
@@ -8755,10 +8755,10 @@
         <v>4.046274144212736</v>
       </c>
       <c r="K146" t="n">
-        <v>-0.07420632821454902</v>
+        <v>0.07420632821454902</v>
       </c>
       <c r="L146" t="n">
-        <v>81.63161310268443</v>
+        <v>106.373059925958</v>
       </c>
       <c r="M146" t="n">
         <v>1.154587940725656</v>
@@ -8815,7 +8815,7 @@
         <v>0.06581318083385509</v>
       </c>
       <c r="L147" t="n">
-        <v>60.75988833555465</v>
+        <v>85.66328674761223</v>
       </c>
       <c r="M147" t="n">
         <v>1.09152987837576</v>
@@ -8872,7 +8872,7 @@
         <v>0.0768971921262897</v>
       </c>
       <c r="L148" t="n">
-        <v>54.07852301050909</v>
+        <v>48.52450294573639</v>
       </c>
       <c r="M148" t="n">
         <v>1.037595971786383</v>
@@ -8929,7 +8929,7 @@
         <v>0.08090991051608559</v>
       </c>
       <c r="L149" t="n">
-        <v>46.50502907010236</v>
+        <v>38.90406120066385</v>
       </c>
       <c r="M149" t="n">
         <v>1.02522958618173</v>
@@ -8986,7 +8986,7 @@
         <v>0.04968615658768155</v>
       </c>
       <c r="L150" t="n">
-        <v>33.8027157890349</v>
+        <v>65.40300502810508</v>
       </c>
       <c r="M150" t="n">
         <v>1.004845569835829</v>
@@ -9043,7 +9043,7 @@
         <v>0.05198816044741231</v>
       </c>
       <c r="L151" t="n">
-        <v>9.479618898039591</v>
+        <v>26.83672866832097</v>
       </c>
       <c r="M151" t="n">
         <v>1.174145664777541</v>
@@ -9100,7 +9100,7 @@
         <v>0.1549414110532054</v>
       </c>
       <c r="L152" t="n">
-        <v>52.84642439855917</v>
+        <v>13.27138507599457</v>
       </c>
       <c r="M152" t="n">
         <v>1.050483808098345</v>
@@ -9154,10 +9154,10 @@
         <v>3.228813908541028</v>
       </c>
       <c r="K153" t="n">
-        <v>-0.06267250382009074</v>
+        <v>0.06267250382009074</v>
       </c>
       <c r="L153" t="n">
-        <v>55.34098900183165</v>
+        <v>75.77441315449484</v>
       </c>
       <c r="M153" t="n">
         <v>1.042829813897674</v>
@@ -9211,10 +9211,10 @@
         <v>3.554760577961515</v>
       </c>
       <c r="K154" t="n">
-        <v>-0.1302202089163533</v>
+        <v>0.1302202089163533</v>
       </c>
       <c r="L154" t="n">
-        <v>71.54202504173385</v>
+        <v>23.42188890511785</v>
       </c>
       <c r="M154" t="n">
         <v>1.061000912976035</v>
@@ -9268,10 +9268,10 @@
         <v>3.946753077724664</v>
       </c>
       <c r="K155" t="n">
-        <v>-0.1835345520486993</v>
+        <v>0.1835345520486993</v>
       </c>
       <c r="L155" t="n">
-        <v>74.23921416397936</v>
+        <v>16.13733531097095</v>
       </c>
       <c r="M155" t="n">
         <v>1.143938087564371</v>
@@ -9325,10 +9325,10 @@
         <v>2.651613764292672</v>
       </c>
       <c r="K156" t="n">
-        <v>-0.09841528253309162</v>
+        <v>0.09841528253309162</v>
       </c>
       <c r="L156" t="n">
-        <v>22.7016836411525</v>
+        <v>17.01975615374169</v>
       </c>
       <c r="M156" t="n">
         <v>1.161443956110336</v>
@@ -9382,10 +9382,10 @@
         <v>3.686044338303158</v>
       </c>
       <c r="K157" t="n">
-        <v>-0.07074591022637799</v>
+        <v>0.07074591022637799</v>
       </c>
       <c r="L157" t="n">
-        <v>66.67618762276553</v>
+        <v>88.47623102691941</v>
       </c>
       <c r="M157" t="n">
         <v>1.118147821934009</v>
@@ -9439,10 +9439,10 @@
         <v>4.115166725326672</v>
       </c>
       <c r="K158" t="n">
-        <v>-0.1367153358291368</v>
+        <v>0.1367153358291368</v>
       </c>
       <c r="L158" t="n">
-        <v>97.64320796791674</v>
+        <v>32.96669917687132</v>
       </c>
       <c r="M158" t="n">
         <v>1.059885685377974</v>
@@ -9499,7 +9499,7 @@
         <v>0.1039861424102037</v>
       </c>
       <c r="L159" t="n">
-        <v>66.89903113886449</v>
+        <v>35.72456929888866</v>
       </c>
       <c r="M159" t="n">
         <v>1.053556876077736</v>
@@ -9556,7 +9556,7 @@
         <v>0.04499873049610165</v>
       </c>
       <c r="L160" t="n">
-        <v>69.07315454681407</v>
+        <v>162.4734188321501</v>
       </c>
       <c r="M160" t="n">
         <v>1.003268651605313</v>
@@ -9613,7 +9613,7 @@
         <v>0.06274447903282331</v>
       </c>
       <c r="L161" t="n">
-        <v>54.4883262672138</v>
+        <v>81.05833491005168</v>
       </c>
       <c r="M161" t="n">
         <v>1.080172301760261</v>
@@ -9670,7 +9670,7 @@
         <v>0.03511791929693451</v>
       </c>
       <c r="L162" t="n">
-        <v>0.8320188067841645</v>
+        <v>3.432858195161812</v>
       </c>
       <c r="M162" t="n">
         <v>1.016424683514935</v>
@@ -9724,10 +9724,10 @@
         <v>0.5610554588381644</v>
       </c>
       <c r="K163" t="n">
-        <v>-0.02183836703996198</v>
+        <v>0.02183836703996198</v>
       </c>
       <c r="L163" t="n">
-        <v>0.3124389648532915</v>
+        <v>3.274346844004153</v>
       </c>
       <c r="M163" t="n">
         <v>1.013460337086076</v>
@@ -9781,10 +9781,10 @@
         <v>0.8109567204545881</v>
       </c>
       <c r="K164" t="n">
-        <v>-0.0305817818706011</v>
+        <v>0.0305817818706011</v>
       </c>
       <c r="L164" t="n">
-        <v>0.7572683358519815</v>
+        <v>5.042142151878857</v>
       </c>
       <c r="M164" t="n">
         <v>1.097137281506887</v>
@@ -9841,7 +9841,7 @@
         <v>0.02143788405185485</v>
       </c>
       <c r="L165" t="n">
-        <v>0.3271229454740646</v>
+        <v>4.052183992340797</v>
       </c>
       <c r="M165" t="n">
         <v>1.06741987687703</v>
@@ -9898,7 +9898,7 @@
         <v>0.02834064342148054</v>
       </c>
       <c r="L166" t="n">
-        <v>0.6303897986939067</v>
+        <v>4.860510143066584</v>
       </c>
       <c r="M166" t="n">
         <v>1.101670904567358</v>
@@ -9952,10 +9952,10 @@
         <v>0.5988416630274465</v>
       </c>
       <c r="K167" t="n">
-        <v>-0.02396645109247175</v>
+        <v>0.02396645109247175</v>
       </c>
       <c r="L167" t="n">
-        <v>0.3304538197441788</v>
+        <v>3.305797076529184</v>
       </c>
       <c r="M167" t="n">
         <v>1.067604665474161</v>
@@ -10009,10 +10009,10 @@
         <v>0.5988416630274465</v>
       </c>
       <c r="K168" t="n">
-        <v>-0.02396645109247175</v>
+        <v>0.02396645109247175</v>
       </c>
       <c r="L168" t="n">
-        <v>0.3304538197441788</v>
+        <v>3.305797076529184</v>
       </c>
       <c r="M168" t="n">
         <v>1.067604665474161</v>
@@ -10069,7 +10069,7 @@
         <v>0.02382992929293667</v>
       </c>
       <c r="L169" t="n">
-        <v>0.4032824762560532</v>
+        <v>3.525139536658912</v>
       </c>
       <c r="M169" t="n">
         <v>1.011989686847492</v>
@@ -10123,10 +10123,10 @@
         <v>0.5771736104287819</v>
       </c>
       <c r="K170" t="n">
-        <v>-0.02284605609048487</v>
+        <v>0.02284605609048487</v>
       </c>
       <c r="L170" t="n">
-        <v>0.3442353647039888</v>
+        <v>3.257200908116733</v>
       </c>
       <c r="M170" t="n">
         <v>1.011994910689844</v>
@@ -10180,10 +10180,10 @@
         <v>0.8154709557086806</v>
       </c>
       <c r="K171" t="n">
-        <v>-0.0372313023840352</v>
+        <v>0.0372313023840352</v>
       </c>
       <c r="L171" t="n">
-        <v>0.965683499506418</v>
+        <v>3.459048586547777</v>
       </c>
       <c r="M171" t="n">
         <v>1.009266852234485</v>
@@ -10240,7 +10240,7 @@
         <v>0.02980997547095671</v>
       </c>
       <c r="L172" t="n">
-        <v>0.5941425042358223</v>
+        <v>3.893179299359939</v>
       </c>
       <c r="M172" t="n">
         <v>1.074374669019925</v>
@@ -10297,7 +10297,7 @@
         <v>0.02529535985636794</v>
       </c>
       <c r="L173" t="n">
-        <v>0.4113792843157314</v>
+        <v>4.023449348760863</v>
       </c>
       <c r="M173" t="n">
         <v>1.097680826244144</v>
@@ -10354,7 +10354,7 @@
         <v>0.07648152833761702</v>
       </c>
       <c r="L174" t="n">
-        <v>3.322494951323657</v>
+        <v>4.105402140332515</v>
       </c>
       <c r="M174" t="n">
         <v>1.157396045992513</v>
@@ -10408,10 +10408,10 @@
         <v>0.9107982991172427</v>
       </c>
       <c r="K175" t="n">
-        <v>-0.03867801685111687</v>
+        <v>0.03867801685111687</v>
       </c>
       <c r="L175" t="n">
-        <v>1.122521090038386</v>
+        <v>4.46566214310221</v>
       </c>
       <c r="M175" t="n">
         <v>1.086161143725312</v>
@@ -10468,7 +10468,7 @@
         <v>0.025506180023759</v>
       </c>
       <c r="L176" t="n">
-        <v>0.3940953332997878</v>
+        <v>4.03428906276426</v>
       </c>
       <c r="M176" t="n">
         <v>1.115686793192477</v>
@@ -10525,7 +10525,7 @@
         <v>0.02208002727165019</v>
       </c>
       <c r="L177" t="n">
-        <v>0.3335309784903651</v>
+        <v>4.767729634707017</v>
       </c>
       <c r="M177" t="n">
         <v>1.142236740101606</v>
@@ -10582,7 +10582,7 @@
         <v>0.01639963361387873</v>
       </c>
       <c r="L178" t="n">
-        <v>0.2074852637186937</v>
+        <v>4.488504765226681</v>
       </c>
       <c r="M178" t="n">
         <v>1.077983570415407</v>
@@ -10639,7 +10639,7 @@
         <v>0.02236647298027311</v>
       </c>
       <c r="L179" t="n">
-        <v>0.3287452062534894</v>
+        <v>4.360445805377414</v>
       </c>
       <c r="M179" t="n">
         <v>1.115050552912205</v>
@@ -10696,7 +10696,7 @@
         <v>0.02248656620456154</v>
       </c>
       <c r="L180" t="n">
-        <v>0.3401625862698531</v>
+        <v>3.724903856631641</v>
       </c>
       <c r="M180" t="n">
         <v>1.06049606874095</v>
@@ -10753,7 +10753,7 @@
         <v>0.03755504426364895</v>
       </c>
       <c r="L181" t="n">
-        <v>0.8804664001014267</v>
+        <v>4.105583628401168</v>
       </c>
       <c r="M181" t="n">
         <v>1.12011900137404</v>
@@ -10807,10 +10807,10 @@
         <v>1.010913520348569</v>
       </c>
       <c r="K182" t="n">
-        <v>-0.05166374143399961</v>
+        <v>0.05166374143399961</v>
       </c>
       <c r="L182" t="n">
-        <v>1.748937364516958</v>
+        <v>3.422298865439287</v>
       </c>
       <c r="M182" t="n">
         <v>1.03307968859881</v>
@@ -10864,10 +10864,10 @@
         <v>0.8063466655782454</v>
       </c>
       <c r="K183" t="n">
-        <v>-0.02868569350378599</v>
+        <v>0.02868569350378599</v>
       </c>
       <c r="L183" t="n">
-        <v>0.7315940147281363</v>
+        <v>5.633551930672652</v>
       </c>
       <c r="M183" t="n">
         <v>1.090067411845544</v>
@@ -10924,7 +10924,7 @@
         <v>0.04988786748610189</v>
       </c>
       <c r="L184" t="n">
-        <v>2.173764227665375</v>
+        <v>4.470691137232148</v>
       </c>
       <c r="M184" t="n">
         <v>1.019755490478512</v>
@@ -10981,7 +10981,7 @@
         <v>0.025577463686609</v>
       </c>
       <c r="L185" t="n">
-        <v>0.831724123260672</v>
+        <v>6.131215580706201</v>
       </c>
       <c r="M185" t="n">
         <v>1.008808594768329</v>
@@ -11035,10 +11035,10 @@
         <v>0.925575594078291</v>
       </c>
       <c r="K186" t="n">
-        <v>-0.03409297133753532</v>
+        <v>0.03409297133753532</v>
       </c>
       <c r="L186" t="n">
-        <v>1.486549164333166</v>
+        <v>6.03189264191931</v>
       </c>
       <c r="M186" t="n">
         <v>1.002729840782555</v>
@@ -11092,10 +11092,10 @@
         <v>1.245715365616588</v>
       </c>
       <c r="K187" t="n">
-        <v>-0.05501792177748832</v>
+        <v>0.05501792177748832</v>
       </c>
       <c r="L187" t="n">
-        <v>2.206441062816467</v>
+        <v>5.646713167562909</v>
       </c>
       <c r="M187" t="n">
         <v>1.167427430458345</v>
@@ -11152,7 +11152,7 @@
         <v>0.02791239717896728</v>
       </c>
       <c r="L188" t="n">
-        <v>0.8400454020009644</v>
+        <v>6.240706935791471</v>
       </c>
       <c r="M188" t="n">
         <v>1.072755420389981</v>
@@ -11206,10 +11206,10 @@
         <v>1.140146777215854</v>
       </c>
       <c r="K189" t="n">
-        <v>-0.05080918398777557</v>
+        <v>0.05080918398777557</v>
       </c>
       <c r="L189" t="n">
-        <v>2.440272473257069</v>
+        <v>5.076278939868278</v>
       </c>
       <c r="M189" t="n">
         <v>1.045089944602988</v>
@@ -11266,7 +11266,7 @@
         <v>0.02788797550161372</v>
       </c>
       <c r="L190" t="n">
-        <v>1.162485332067964</v>
+        <v>8.604408946162458</v>
       </c>
       <c r="M190" t="n">
         <v>1.06862931220776</v>
@@ -11320,10 +11320,10 @@
         <v>0.6650521316187403</v>
       </c>
       <c r="K191" t="n">
-        <v>-0.01469478283644105</v>
+        <v>0.01469478283644105</v>
       </c>
       <c r="L191" t="n">
-        <v>0.3243748409814904</v>
+        <v>12.04448822150114</v>
       </c>
       <c r="M191" t="n">
         <v>1.194664520776338</v>
@@ -11377,10 +11377,10 @@
         <v>1.049385183707868</v>
       </c>
       <c r="K192" t="n">
-        <v>-0.04456879856407352</v>
+        <v>0.04456879856407352</v>
       </c>
       <c r="L192" t="n">
-        <v>1.859157766135297</v>
+        <v>5.143876781549639</v>
       </c>
       <c r="M192" t="n">
         <v>1.045664303179204</v>
@@ -11434,10 +11434,10 @@
         <v>0.9563546516654242</v>
       </c>
       <c r="K193" t="n">
-        <v>-0.04332297250611448</v>
+        <v>0.04332297250611448</v>
       </c>
       <c r="L193" t="n">
-        <v>1.528059903141882</v>
+        <v>4.120672090202204</v>
       </c>
       <c r="M193" t="n">
         <v>1.025639197322044</v>
@@ -11494,7 +11494,7 @@
         <v>0.02120983171356979</v>
       </c>
       <c r="L194" t="n">
-        <v>0.7084559041365309</v>
+        <v>7.522627033999032</v>
       </c>
       <c r="M194" t="n">
         <v>1.007831653687972</v>
@@ -11548,10 +11548,10 @@
         <v>0.9380855904213254</v>
       </c>
       <c r="K195" t="n">
-        <v>-0.03205106725063669</v>
+        <v>0.03205106725063669</v>
       </c>
       <c r="L195" t="n">
-        <v>1.014774401269705</v>
+        <v>7.105424524474869</v>
       </c>
       <c r="M195" t="n">
         <v>1.15360514059645</v>
@@ -11608,7 +11608,7 @@
         <v>0.03655590562710845</v>
       </c>
       <c r="L196" t="n">
-        <v>1.228664638404857</v>
+        <v>6.786076237485717</v>
       </c>
       <c r="M196" t="n">
         <v>1.121307806079401</v>
@@ -11665,7 +11665,7 @@
         <v>0.02821641145481779</v>
       </c>
       <c r="L197" t="n">
-        <v>0.8040573822728589</v>
+        <v>6.742586931220517</v>
       </c>
       <c r="M197" t="n">
         <v>1.087704603360696</v>
@@ -11722,7 +11722,7 @@
         <v>0.03556881785644881</v>
       </c>
       <c r="L198" t="n">
-        <v>1.307465857262395</v>
+        <v>6.197159185778193</v>
       </c>
       <c r="M198" t="n">
         <v>1.088645104106979</v>
@@ -11779,7 +11779,7 @@
         <v>0.030474447992722</v>
       </c>
       <c r="L199" t="n">
-        <v>0.9488491512782431</v>
+        <v>6.40806155147355</v>
       </c>
       <c r="M199" t="n">
         <v>1.106451230639899</v>
@@ -11833,10 +11833,10 @@
         <v>0.8293715379859978</v>
       </c>
       <c r="K200" t="n">
-        <v>-0.02811591008932707</v>
+        <v>0.02811591008932707</v>
       </c>
       <c r="L200" t="n">
-        <v>0.8914167734783959</v>
+        <v>6.381028978760989</v>
       </c>
       <c r="M200" t="n">
         <v>1.058990595005114</v>
@@ -11893,7 +11893,7 @@
         <v>0.03010618523789385</v>
       </c>
       <c r="L201" t="n">
-        <v>0.9099043183806114</v>
+        <v>7.337640892675374</v>
       </c>
       <c r="M201" t="n">
         <v>1.15769984520877</v>
@@ -11950,7 +11950,7 @@
         <v>0.007645123593210006</v>
       </c>
       <c r="L202" t="n">
-        <v>0.2473946874836379</v>
+        <v>42.30878145525282</v>
       </c>
       <c r="M202" t="n">
         <v>1.292008495732944</v>
@@ -12004,10 +12004,10 @@
         <v>0.3364031263141598</v>
       </c>
       <c r="K203" t="n">
-        <v>-0.003628220134123581</v>
+        <v>0.003628220134123581</v>
       </c>
       <c r="L203" t="n">
-        <v>0.05394262268155392</v>
+        <v>25.57057170558073</v>
       </c>
       <c r="M203" t="n">
         <v>1.0918463122622</v>
@@ -12064,7 +12064,7 @@
         <v>0.003101091194403563</v>
       </c>
       <c r="L204" t="n">
-        <v>0.03873113142153875</v>
+        <v>29.0418803217278</v>
       </c>
       <c r="M204" t="n">
         <v>1.158914569047725</v>
@@ -12121,7 +12121,7 @@
         <v>0.006206038739432804</v>
       </c>
       <c r="L205" t="n">
-        <v>0.26735420803884</v>
+        <v>45.74924131909913</v>
       </c>
       <c r="M205" t="n">
         <v>1.123730394386707</v>
@@ -12178,7 +12178,7 @@
         <v>0.006603833457227455</v>
       </c>
       <c r="L206" t="n">
-        <v>0.1595479678957466</v>
+        <v>24.70968483053875</v>
       </c>
       <c r="M206" t="n">
         <v>1.127988226796963</v>
@@ -12235,7 +12235,7 @@
         <v>0.00191294429231937</v>
       </c>
       <c r="L207" t="n">
-        <v>0.01220817827868607</v>
+        <v>15.60805053742439</v>
       </c>
       <c r="M207" t="n">
         <v>1.002084727855985</v>
@@ -12289,10 +12289,10 @@
         <v>0.1599999189898187</v>
       </c>
       <c r="K208" t="n">
-        <v>-0.001559445159121036</v>
+        <v>0.001559445159121036</v>
       </c>
       <c r="L208" t="n">
-        <v>0.007820148311882366</v>
+        <v>14.89246889583017</v>
       </c>
       <c r="M208" t="n">
         <v>1.000024309958035</v>
@@ -12349,7 +12349,7 @@
         <v>0.004401238285257467</v>
       </c>
       <c r="L209" t="n">
-        <v>0.1071073437189437</v>
+        <v>34.37352825331214</v>
       </c>
       <c r="M209" t="n">
         <v>1.099080226310749</v>
@@ -12403,10 +12403,10 @@
         <v>0.2691168038921695</v>
       </c>
       <c r="K210" t="n">
-        <v>-0.002714575629879689</v>
+        <v>0.002714575629879689</v>
       </c>
       <c r="L210" t="n">
-        <v>0.03715073504529295</v>
+        <v>23.38655132849739</v>
       </c>
       <c r="M210" t="n">
         <v>1.00032941092064</v>
@@ -12463,7 +12463,7 @@
         <v>0.009502633669377369</v>
       </c>
       <c r="L211" t="n">
-        <v>0.3111251154141131</v>
+        <v>35.42928068121873</v>
       </c>
       <c r="M211" t="n">
         <v>1.304415347939527</v>
@@ -12517,10 +12517,10 @@
         <v>0.2559630921600582</v>
       </c>
       <c r="K212" t="n">
-        <v>-0.002709000402212257</v>
+        <v>0.002709000402212257</v>
       </c>
       <c r="L212" t="n">
-        <v>0.03099457394785406</v>
+        <v>20.20512453469297</v>
       </c>
       <c r="M212" t="n">
         <v>1.000622621305699</v>
@@ -12574,10 +12574,10 @@
         <v>0.1280308497310249</v>
       </c>
       <c r="K213" t="n">
-        <v>-0.001170002407538374</v>
+        <v>0.001170002407538374</v>
       </c>
       <c r="L213" t="n">
-        <v>0.003958869058538636</v>
+        <v>13.55557672206339</v>
       </c>
       <c r="M213" t="n">
         <v>1.00069879038756</v>
@@ -12634,7 +12634,7 @@
         <v>0.001889649816095974</v>
       </c>
       <c r="L214" t="n">
-        <v>0.01475423339072421</v>
+        <v>19.20358299903283</v>
       </c>
       <c r="M214" t="n">
         <v>1.0012789506589</v>
@@ -12691,7 +12691,7 @@
         <v>0.00886575262867903</v>
       </c>
       <c r="L215" t="n">
-        <v>0.2732687961032371</v>
+        <v>34.83992445319648</v>
       </c>
       <c r="M215" t="n">
         <v>1.293072394600371</v>
@@ -12748,7 +12748,7 @@
         <v>0.002745221330212041</v>
       </c>
       <c r="L216" t="n">
-        <v>0.03070165757188474</v>
+        <v>19.90487977442061</v>
       </c>
       <c r="M216" t="n">
         <v>1.003682488897184</v>
@@ -12805,7 +12805,7 @@
         <v>0.01018634526584732</v>
       </c>
       <c r="L217" t="n">
-        <v>0.6140298277924028</v>
+        <v>51.60633169215366</v>
       </c>
       <c r="M217" t="n">
         <v>1.15857862261441</v>
@@ -12859,10 +12859,10 @@
         <v>0.6888056522164214</v>
       </c>
       <c r="K218" t="n">
-        <v>-0.009104348979667939</v>
+        <v>0.009104348979667939</v>
       </c>
       <c r="L218" t="n">
-        <v>0.2813634236160566</v>
+        <v>34.86100799494563</v>
       </c>
       <c r="M218" t="n">
         <v>1.303741623922343</v>
@@ -12916,10 +12916,10 @@
         <v>0.1446694851249118</v>
       </c>
       <c r="K219" t="n">
-        <v>-0.001249885838623954</v>
+        <v>0.001249885838623954</v>
       </c>
       <c r="L219" t="n">
-        <v>0.005663112263646982</v>
+        <v>17.13711610299849</v>
       </c>
       <c r="M219" t="n">
         <v>1.000000586759297</v>
@@ -12973,10 +12973,10 @@
         <v>0.2553412106884184</v>
       </c>
       <c r="K220" t="n">
-        <v>-0.002985145673043122</v>
+        <v>0.002985145673043122</v>
       </c>
       <c r="L220" t="n">
-        <v>0.03147374560540693</v>
+        <v>16.51883091275995</v>
       </c>
       <c r="M220" t="n">
         <v>1.000087852478782</v>
@@ -13033,7 +13033,7 @@
         <v>0.001981113743969378</v>
       </c>
       <c r="L221" t="n">
-        <v>0.01265377675520103</v>
+        <v>15.09586533849213</v>
       </c>
       <c r="M221" t="n">
         <v>1.00176827886891</v>
@@ -13090,7 +13090,7 @@
         <v>0.0253680159222087</v>
       </c>
       <c r="L222" t="n">
-        <v>0.9302521824870439</v>
+        <v>7.321349061993596</v>
       </c>
       <c r="M222" t="n">
         <v>1.030284542594431</v>
@@ -13147,7 +13147,7 @@
         <v>0.04240807096871236</v>
       </c>
       <c r="L223" t="n">
-        <v>2.28556825042204</v>
+        <v>5.943893930620487</v>
       </c>
       <c r="M223" t="n">
         <v>1.003403805436125</v>
@@ -13201,10 +13201,10 @@
         <v>1.476727765124769</v>
       </c>
       <c r="K224" t="n">
-        <v>-0.06731719958169924</v>
+        <v>0.06731719958169924</v>
       </c>
       <c r="L224" t="n">
-        <v>5.743738084550275</v>
+        <v>6.283431229223153</v>
       </c>
       <c r="M224" t="n">
         <v>1.007106985709629</v>
@@ -13261,7 +13261,7 @@
         <v>0.04970180234443927</v>
       </c>
       <c r="L225" t="n">
-        <v>2.97740185527176</v>
+        <v>7.633093968052767</v>
       </c>
       <c r="M225" t="n">
         <v>1.110069676585527</v>
@@ -13318,7 +13318,7 @@
         <v>0.03089175316362942</v>
       </c>
       <c r="L226" t="n">
-        <v>1.404328545947438</v>
+        <v>7.076897101132859</v>
       </c>
       <c r="M226" t="n">
         <v>1.010690423871112</v>
@@ -13372,10 +13372,10 @@
         <v>0.9370096037588547</v>
       </c>
       <c r="K227" t="n">
-        <v>-0.03568422905621716</v>
+        <v>0.03568422905621716</v>
       </c>
       <c r="L227" t="n">
-        <v>1.53890547185042</v>
+        <v>5.712511878473634</v>
       </c>
       <c r="M227" t="n">
         <v>1.006504465197547</v>
@@ -13432,7 +13432,7 @@
         <v>0.02808990888051375</v>
       </c>
       <c r="L228" t="n">
-        <v>1.063467472140194</v>
+        <v>6.815640186601542</v>
       </c>
       <c r="M228" t="n">
         <v>1.029838037147323</v>
@@ -13489,7 +13489,7 @@
         <v>0.04600145240084352</v>
       </c>
       <c r="L229" t="n">
-        <v>3.055180306111803</v>
+        <v>11.03399063831088</v>
       </c>
       <c r="M229" t="n">
         <v>1.174535508136058</v>
@@ -13543,10 +13543,10 @@
         <v>1.664405447512864</v>
       </c>
       <c r="K230" t="n">
-        <v>-0.05918968783418128</v>
+        <v>0.05918968783418128</v>
       </c>
       <c r="L230" t="n">
-        <v>5.696763068010876</v>
+        <v>11.63678239386247</v>
       </c>
       <c r="M230" t="n">
         <v>1.121741200451573</v>
@@ -13600,10 +13600,10 @@
         <v>0.9604677125615786</v>
       </c>
       <c r="K231" t="n">
-        <v>-0.02510138625067001</v>
+        <v>0.02510138625067001</v>
       </c>
       <c r="L231" t="n">
-        <v>1.437003873142082</v>
+        <v>12.43370398266923</v>
       </c>
       <c r="M231" t="n">
         <v>1.049475409307415</v>
@@ -13660,7 +13660,7 @@
         <v>0.08358064303469578</v>
       </c>
       <c r="L232" t="n">
-        <v>6.174160201203853</v>
+        <v>6.066581658286434</v>
       </c>
       <c r="M232" t="n">
         <v>1.139585995655979</v>
@@ -13717,7 +13717,7 @@
         <v>0.02328468352472924</v>
       </c>
       <c r="L233" t="n">
-        <v>1.344440686222973</v>
+        <v>12.36784211192983</v>
       </c>
       <c r="M233" t="n">
         <v>1.021784756409177</v>
@@ -13774,7 +13774,7 @@
         <v>0.02756015218434255</v>
       </c>
       <c r="L234" t="n">
-        <v>1.555491481441613</v>
+        <v>11.71585637307851</v>
       </c>
       <c r="M234" t="n">
         <v>1.068741243999049</v>
@@ -13828,10 +13828,10 @@
         <v>0.9678257069435777</v>
       </c>
       <c r="K235" t="n">
-        <v>-0.02541541336412107</v>
+        <v>0.02541541336412107</v>
       </c>
       <c r="L235" t="n">
-        <v>1.548679613702763</v>
+        <v>12.40922707441872</v>
       </c>
       <c r="M235" t="n">
         <v>1.036294012415398</v>
@@ -13888,7 +13888,7 @@
         <v>0.03253927282538442</v>
       </c>
       <c r="L236" t="n">
-        <v>1.924871965506583</v>
+        <v>11.51712527102112</v>
       </c>
       <c r="M236" t="n">
         <v>1.110189589640596</v>
@@ -13942,10 +13942,10 @@
         <v>0.988637057024689</v>
       </c>
       <c r="K237" t="n">
-        <v>-0.02681562350397914</v>
+        <v>0.02681562350397914</v>
       </c>
       <c r="L237" t="n">
-        <v>1.583719086651124</v>
+        <v>11.88180670377196</v>
       </c>
       <c r="M237" t="n">
         <v>1.051374486045056</v>
@@ -14002,7 +14002,7 @@
         <v>0.02542601934908376</v>
       </c>
       <c r="L238" t="n">
-        <v>1.530111716198731</v>
+        <v>12.19489084833966</v>
       </c>
       <c r="M238" t="n">
         <v>1.036051619663672</v>
@@ -14056,10 +14056,10 @@
         <v>0.6412671162423895</v>
       </c>
       <c r="K239" t="n">
-        <v>-0.01945197360457841</v>
+        <v>0.01945197360457841</v>
       </c>
       <c r="L239" t="n">
-        <v>0.4912139321346878</v>
+        <v>6.162219924064127</v>
       </c>
       <c r="M239" t="n">
         <v>1.005958872040124</v>
@@ -14113,10 +14113,10 @@
         <v>1.069845506153562</v>
       </c>
       <c r="K240" t="n">
-        <v>-0.04446503774060799</v>
+        <v>0.04446503774060799</v>
       </c>
       <c r="L240" t="n">
-        <v>2.057808476679439</v>
+        <v>5.476126808202708</v>
       </c>
       <c r="M240" t="n">
         <v>1.043501483377437</v>
@@ -14170,10 +14170,10 @@
         <v>0.9627853703206588</v>
       </c>
       <c r="K241" t="n">
-        <v>-0.03461784314982667</v>
+        <v>0.03461784314982667</v>
       </c>
       <c r="L241" t="n">
-        <v>1.380854223153455</v>
+        <v>6.584701047043095</v>
       </c>
       <c r="M241" t="n">
         <v>1.072412211302558</v>
@@ -14230,7 +14230,7 @@
         <v>0.01021670916946873</v>
       </c>
       <c r="L242" t="n">
-        <v>0.303929837741017</v>
+        <v>13.94805365474747</v>
       </c>
       <c r="M242" t="n">
         <v>1.005866013365425</v>
@@ -14284,10 +14284,10 @@
         <v>0.5419660622389222</v>
       </c>
       <c r="K243" t="n">
-        <v>-0.01082784414689905</v>
+        <v>0.01082784414689905</v>
       </c>
       <c r="L243" t="n">
-        <v>0.2908374379628063</v>
+        <v>12.00549055648382</v>
       </c>
       <c r="M243" t="n">
         <v>1.008839883344032</v>
@@ -14344,7 +14344,7 @@
         <v>0.01741517325459946</v>
       </c>
       <c r="L244" t="n">
-        <v>0.5034435407804462</v>
+        <v>9.843058422038101</v>
       </c>
       <c r="M244" t="n">
         <v>1.005876697968441</v>
@@ -14398,10 +14398,10 @@
         <v>0.6642781061901795</v>
       </c>
       <c r="K245" t="n">
-        <v>-0.01733410616231071</v>
+        <v>0.01733410616231071</v>
       </c>
       <c r="L245" t="n">
-        <v>0.4495594061912575</v>
+        <v>8.62570376507745</v>
       </c>
       <c r="M245" t="n">
         <v>1.006941288413395</v>
@@ -14458,7 +14458,7 @@
         <v>0.02279971241659657</v>
       </c>
       <c r="L246" t="n">
-        <v>0.6931932006929338</v>
+        <v>6.352793518692661</v>
       </c>
       <c r="M246" t="n">
         <v>1.005599311326732</v>
@@ -14515,7 +14515,7 @@
         <v>0.02221053777099249</v>
       </c>
       <c r="L247" t="n">
-        <v>0.6366751717941722</v>
+        <v>11.56125652753709</v>
       </c>
       <c r="M247" t="n">
         <v>1.218295695311843</v>
@@ -14569,10 +14569,10 @@
         <v>1.254018520256235</v>
       </c>
       <c r="K248" t="n">
-        <v>-0.03840096394247714</v>
+        <v>0.03840096394247714</v>
       </c>
       <c r="L248" t="n">
-        <v>1.717663363690425</v>
+        <v>11.82429416936601</v>
       </c>
       <c r="M248" t="n">
         <v>1.293888446367377</v>
@@ -14629,7 +14629,7 @@
         <v>0.02493524799487245</v>
       </c>
       <c r="L249" t="n">
-        <v>0.8095813241048926</v>
+        <v>9.47578168517505</v>
       </c>
       <c r="M249" t="n">
         <v>1.157509249321573</v>
@@ -14686,7 +14686,7 @@
         <v>0.01947153059385788</v>
       </c>
       <c r="L250" t="n">
-        <v>0.5995886775092875</v>
+        <v>11.35193332684438</v>
       </c>
       <c r="M250" t="n">
         <v>1.153724898325228</v>
@@ -14743,7 +14743,7 @@
         <v>0.05720854437619411</v>
       </c>
       <c r="L251" t="n">
-        <v>2.266256074508967</v>
+        <v>5.556862861146736</v>
       </c>
       <c r="M251" t="n">
         <v>1.197062284716925</v>
@@ -14800,7 +14800,7 @@
         <v>0.0121057851742202</v>
       </c>
       <c r="L252" t="n">
-        <v>0.3381545949454081</v>
+        <v>10.90131121743787</v>
       </c>
       <c r="M252" t="n">
         <v>1.003138334358944</v>
@@ -14857,7 +14857,7 @@
         <v>0.01542475068123313</v>
       </c>
       <c r="L253" t="n">
-        <v>0.4330159063659489</v>
+        <v>8.833890274504375</v>
       </c>
       <c r="M253" t="n">
         <v>1.008304572533728</v>
@@ -14911,10 +14911,10 @@
         <v>0.576236517965498</v>
       </c>
       <c r="K254" t="n">
-        <v>-0.01174038261270323</v>
+        <v>0.01174038261270323</v>
       </c>
       <c r="L254" t="n">
-        <v>0.3535339683065301</v>
+        <v>12.27398131424196</v>
       </c>
       <c r="M254" t="n">
         <v>1.006514480718194</v>
@@ -14968,10 +14968,10 @@
         <v>0.6002368786434605</v>
       </c>
       <c r="K255" t="n">
-        <v>-0.01326044454745692</v>
+        <v>0.01326044454745692</v>
       </c>
       <c r="L255" t="n">
-        <v>0.3603400226355345</v>
+        <v>10.87425427871887</v>
       </c>
       <c r="M255" t="n">
         <v>1.021767136665372</v>
@@ -15028,7 +15028,7 @@
         <v>0.01354429074940131</v>
       </c>
       <c r="L256" t="n">
-        <v>0.3713049655499687</v>
+        <v>10.94287796149884</v>
       </c>
       <c r="M256" t="n">
         <v>1.023729808492647</v>
@@ -15082,10 +15082,10 @@
         <v>0.6929656481643166</v>
       </c>
       <c r="K257" t="n">
-        <v>-0.01932879934195772</v>
+        <v>0.01932879934195772</v>
       </c>
       <c r="L257" t="n">
-        <v>0.6180320039393922</v>
+        <v>7.875406687154378</v>
       </c>
       <c r="M257" t="n">
         <v>1.003630201373164</v>
@@ -15139,10 +15139,10 @@
         <v>0.6555431956721041</v>
       </c>
       <c r="K258" t="n">
-        <v>-0.01529087697453267</v>
+        <v>0.01529087697453267</v>
       </c>
       <c r="L258" t="n">
-        <v>0.5209348436303212</v>
+        <v>10.65336434184406</v>
       </c>
       <c r="M258" t="n">
         <v>1.01053439938411</v>
@@ -15196,10 +15196,10 @@
         <v>0.6032847186994105</v>
       </c>
       <c r="K259" t="n">
-        <v>-0.01417866197309545</v>
+        <v>0.01417866197309545</v>
       </c>
       <c r="L259" t="n">
-        <v>0.4137864401038</v>
+        <v>9.657041617247533</v>
       </c>
       <c r="M259" t="n">
         <v>1.004057842779753</v>
@@ -15253,10 +15253,10 @@
         <v>0.4930077049932141</v>
       </c>
       <c r="K260" t="n">
-        <v>-0.009026614556400548</v>
+        <v>0.009026614556400548</v>
       </c>
       <c r="L260" t="n">
-        <v>0.2241404126763598</v>
+        <v>13.00346072920875</v>
       </c>
       <c r="M260" t="n">
         <v>1.006721555709741</v>
@@ -15310,10 +15310,10 @@
         <v>0.4787054023083315</v>
       </c>
       <c r="K261" t="n">
-        <v>-0.008871766474268839</v>
+        <v>0.008871766474268839</v>
       </c>
       <c r="L261" t="n">
-        <v>0.2051220337650927</v>
+        <v>12.32345288830669</v>
       </c>
       <c r="M261" t="n">
         <v>1.006820125440015</v>
@@ -15370,7 +15370,7 @@
         <v>0.4248289631907749</v>
       </c>
       <c r="L262" t="n">
-        <v>39.38934931282382</v>
+        <v>2.2017016457322</v>
       </c>
       <c r="M262" t="n">
         <v>1.265266576947335</v>
@@ -15424,10 +15424,10 @@
         <v>3.633457041342867</v>
       </c>
       <c r="K263" t="n">
-        <v>-0.4414321384610088</v>
+        <v>0.4414321384610088</v>
       </c>
       <c r="L263" t="n">
-        <v>40.50662469917403</v>
+        <v>2.176605982718548</v>
       </c>
       <c r="M263" t="n">
         <v>1.281071141579463</v>
@@ -15481,10 +15481,10 @@
         <v>3.610990151651357</v>
       </c>
       <c r="K264" t="n">
-        <v>-0.4402273842594943</v>
+        <v>0.4402273842594943</v>
       </c>
       <c r="L264" t="n">
-        <v>39.91534535536846</v>
+        <v>2.148188710651276</v>
       </c>
       <c r="M264" t="n">
         <v>1.279405373564848</v>
@@ -15541,7 +15541,7 @@
         <v>0.2301882253236948</v>
       </c>
       <c r="L265" t="n">
-        <v>22.11574776347404</v>
+        <v>2.310134604865937</v>
       </c>
       <c r="M265" t="n">
         <v>1.06120701660683</v>
@@ -15598,7 +15598,7 @@
         <v>0.2019289107430968</v>
       </c>
       <c r="L266" t="n">
-        <v>17.81798814837474</v>
+        <v>2.413799616571475</v>
       </c>
       <c r="M266" t="n">
         <v>1.01247969353119</v>
@@ -15655,7 +15655,7 @@
         <v>0.4038868450979878</v>
       </c>
       <c r="L267" t="n">
-        <v>34.09564804217923</v>
+        <v>2.033345955527714</v>
       </c>
       <c r="M267" t="n">
         <v>1.242599685506609</v>
@@ -15712,7 +15712,7 @@
         <v>0.2318402319417754</v>
       </c>
       <c r="L268" t="n">
-        <v>18.49317283337752</v>
+        <v>2.376907641550676</v>
       </c>
       <c r="M268" t="n">
         <v>1.142731181981387</v>
@@ -15766,10 +15766,10 @@
         <v>3.592562695189673</v>
       </c>
       <c r="K269" t="n">
-        <v>-0.441572398442827</v>
+        <v>0.441572398442827</v>
       </c>
       <c r="L269" t="n">
-        <v>39.41178865808564</v>
+        <v>2.102600950487701</v>
       </c>
       <c r="M269" t="n">
         <v>1.278274874214713</v>
@@ -15823,10 +15823,10 @@
         <v>3.55664433706047</v>
       </c>
       <c r="K270" t="n">
-        <v>-0.4283491041125739</v>
+        <v>0.4283491041125739</v>
       </c>
       <c r="L270" t="n">
-        <v>39.26140292970258</v>
+        <v>2.168069575256347</v>
       </c>
       <c r="M270" t="n">
         <v>1.267108219322657</v>
@@ -15880,10 +15880,10 @@
         <v>3.531443680454462</v>
       </c>
       <c r="K271" t="n">
-        <v>-0.422423053292324</v>
+        <v>0.422423053292324</v>
       </c>
       <c r="L271" t="n">
-        <v>38.92555833494623</v>
+        <v>2.18227389421071</v>
       </c>
       <c r="M271" t="n">
         <v>1.261738555601919</v>
@@ -15937,10 +15937,10 @@
         <v>3.193468386137244</v>
       </c>
       <c r="K272" t="n">
-        <v>-0.3055453575214225</v>
+        <v>0.3055453575214225</v>
       </c>
       <c r="L272" t="n">
-        <v>32.25359917483986</v>
+        <v>3.084495289403613</v>
       </c>
       <c r="M272" t="n">
         <v>1.211523504748349</v>
@@ -15997,7 +15997,7 @@
         <v>0.3279926779090434</v>
       </c>
       <c r="L273" t="n">
-        <v>26.47501751197969</v>
+        <v>2.146925443822357</v>
       </c>
       <c r="M273" t="n">
         <v>1.19203337163804</v>
@@ -16051,10 +16051,10 @@
         <v>3.094658171716357</v>
       </c>
       <c r="K274" t="n">
-        <v>-0.2889859654530229</v>
+        <v>0.2889859654530229</v>
       </c>
       <c r="L274" t="n">
-        <v>30.98470410244974</v>
+        <v>3.137849989949947</v>
       </c>
       <c r="M274" t="n">
         <v>1.189849873406192</v>
@@ -16111,7 +16111,7 @@
         <v>0.5027752546002777</v>
       </c>
       <c r="L275" t="n">
-        <v>42.88589105257065</v>
+        <v>2.397522969139299</v>
       </c>
       <c r="M275" t="n">
         <v>1.450607637262168</v>
@@ -16168,7 +16168,7 @@
         <v>0.4248287178364803</v>
       </c>
       <c r="L276" t="n">
-        <v>39.38930700545374</v>
+        <v>2.20170191922978</v>
       </c>
       <c r="M276" t="n">
         <v>1.265266303299498</v>
@@ -16222,10 +16222,10 @@
         <v>1.929629282971872</v>
       </c>
       <c r="K277" t="n">
-        <v>-0.1777295625094594</v>
+        <v>0.1777295625094594</v>
       </c>
       <c r="L277" t="n">
-        <v>9.698844873253893</v>
+        <v>2.011175297937823</v>
       </c>
       <c r="M277" t="n">
         <v>1.07599062839611</v>
@@ -16279,10 +16279,10 @@
         <v>2.824032746672052</v>
       </c>
       <c r="K278" t="n">
-        <v>-0.3385684987748244</v>
+        <v>0.3385684987748244</v>
       </c>
       <c r="L278" t="n">
-        <v>32.34933886603312</v>
+        <v>1.737255582525344</v>
       </c>
       <c r="M278" t="n">
         <v>1.098118241253245</v>
@@ -16339,7 +16339,7 @@
         <v>0.3025287036766829</v>
       </c>
       <c r="L279" t="n">
-        <v>25.2803120482668</v>
+        <v>1.929807831820177</v>
       </c>
       <c r="M279" t="n">
         <v>1.118152464512177</v>
@@ -16393,10 +16393,10 @@
         <v>3.193464429980169</v>
       </c>
       <c r="K280" t="n">
-        <v>-0.3055446620604615</v>
+        <v>0.3055446620604615</v>
       </c>
       <c r="L280" t="n">
-        <v>32.25351966522487</v>
+        <v>3.084497867363673</v>
       </c>
       <c r="M280" t="n">
         <v>1.211523041049767</v>
@@ -16453,7 +16453,7 @@
         <v>0.5027749019605429</v>
       </c>
       <c r="L281" t="n">
-        <v>42.88584054589181</v>
+        <v>2.397521730574491</v>
       </c>
       <c r="M281" t="n">
         <v>1.450607278635498</v>
@@ -16510,7 +16510,7 @@
         <v>0.01311313845200324</v>
       </c>
       <c r="L282" t="n">
-        <v>0.3786631280659774</v>
+        <v>10.59786379968241</v>
       </c>
       <c r="M282" t="n">
         <v>1.012948815318994</v>
@@ -16567,7 +16567,7 @@
         <v>0.01578540229800592</v>
       </c>
       <c r="L283" t="n">
-        <v>0.5953037228901301</v>
+        <v>13.06671362024828</v>
       </c>
       <c r="M283" t="n">
         <v>1.056133898147704</v>
@@ -16624,7 +16624,7 @@
         <v>0.05784405835500912</v>
       </c>
       <c r="L284" t="n">
-        <v>3.673770433167582</v>
+        <v>7.239689639903092</v>
       </c>
       <c r="M284" t="n">
         <v>1.022174101737862</v>
@@ -16681,7 +16681,7 @@
         <v>0.003206379555914871</v>
       </c>
       <c r="L285" t="n">
-        <v>0.01980323245898291</v>
+        <v>13.43557892098524</v>
       </c>
       <c r="M285" t="n">
         <v>1.107720077799041</v>
@@ -16735,10 +16735,10 @@
         <v>0.9532571734390621</v>
       </c>
       <c r="K286" t="n">
-        <v>-0.03352086157695455</v>
+        <v>0.03352086157695455</v>
       </c>
       <c r="L286" t="n">
-        <v>1.055132312163432</v>
+        <v>6.81628165479535</v>
       </c>
       <c r="M286" t="n">
         <v>1.115581770803451</v>
@@ -16792,10 +16792,10 @@
         <v>0.60553149814753</v>
       </c>
       <c r="K287" t="n">
-        <v>-0.009408729275406608</v>
+        <v>0.009408729275406608</v>
       </c>
       <c r="L287" t="n">
-        <v>0.3012658683233326</v>
+        <v>22.17664775866915</v>
       </c>
       <c r="M287" t="n">
         <v>1.104825068230446</v>
@@ -16849,10 +16849,10 @@
         <v>1.112621144629525</v>
       </c>
       <c r="K288" t="n">
-        <v>-0.03291389844378802</v>
+        <v>0.03291389844378802</v>
       </c>
       <c r="L288" t="n">
-        <v>2.10278633354945</v>
+        <v>11.24167186522338</v>
       </c>
       <c r="M288" t="n">
         <v>1.040770863832561</v>
@@ -16909,7 +16909,7 @@
         <v>0.01590748132458927</v>
       </c>
       <c r="L289" t="n">
-        <v>0.4590832449513716</v>
+        <v>14.59615338257594</v>
       </c>
       <c r="M289" t="n">
         <v>1.199577083616598</v>
@@ -16963,10 +16963,10 @@
         <v>0.7965123785500041</v>
       </c>
       <c r="K290" t="n">
-        <v>-0.02628333741769262</v>
+        <v>0.02628333741769262</v>
       </c>
       <c r="L290" t="n">
-        <v>0.5212971051780069</v>
+        <v>6.467913367861855</v>
       </c>
       <c r="M290" t="n">
         <v>1.226077037927465</v>
@@ -17023,7 +17023,7 @@
         <v>0.01929752586402047</v>
       </c>
       <c r="L291" t="n">
-        <v>0.4269479581820192</v>
+        <v>7.027476845943383</v>
       </c>
       <c r="M291" t="n">
         <v>1.092258778076547</v>
@@ -17080,7 +17080,7 @@
         <v>0.04590608251148082</v>
       </c>
       <c r="L292" t="n">
-        <v>2.75969791006378</v>
+        <v>9.371847610608036</v>
       </c>
       <c r="M292" t="n">
         <v>1.115128381940253</v>
@@ -17137,7 +17137,7 @@
         <v>0.0240468574364224</v>
       </c>
       <c r="L293" t="n">
-        <v>0.6255716574422349</v>
+        <v>5.174506800176011</v>
       </c>
       <c r="M293" t="n">
         <v>1.010661991065529</v>
@@ -17191,10 +17191,10 @@
         <v>0.9632145896591159</v>
       </c>
       <c r="K294" t="n">
-        <v>-0.03217406676233731</v>
+        <v>0.03217406676233731</v>
       </c>
       <c r="L294" t="n">
-        <v>1.561970642715024</v>
+        <v>7.633168785949802</v>
       </c>
       <c r="M294" t="n">
         <v>1.016061513742064</v>
@@ -17248,10 +17248,10 @@
         <v>1.173291252476692</v>
       </c>
       <c r="K295" t="n">
-        <v>-0.03281070446191971</v>
+        <v>0.03281070446191971</v>
       </c>
       <c r="L295" t="n">
-        <v>2.285732627362886</v>
+        <v>13.265817394292</v>
       </c>
       <c r="M295" t="n">
         <v>1.081479817971211</v>
@@ -17305,10 +17305,10 @@
         <v>1.609407761771963</v>
       </c>
       <c r="K296" t="n">
-        <v>-0.04427689835007648</v>
+        <v>0.04427689835007648</v>
       </c>
       <c r="L296" t="n">
-        <v>5.272163486809277</v>
+        <v>18.80145762264129</v>
       </c>
       <c r="M296" t="n">
         <v>1.058542763642762</v>
@@ -17362,10 +17362,10 @@
         <v>0.9819840414150003</v>
       </c>
       <c r="K297" t="n">
-        <v>-0.03393234673629882</v>
+        <v>0.03393234673629882</v>
       </c>
       <c r="L297" t="n">
-        <v>1.786036346209823</v>
+        <v>7.271652626864634</v>
       </c>
       <c r="M297" t="n">
         <v>1.003866345750728</v>
@@ -17419,10 +17419,10 @@
         <v>0.9568785346896401</v>
       </c>
       <c r="K298" t="n">
-        <v>-0.03203657689340927</v>
+        <v>0.03203657689340927</v>
       </c>
       <c r="L298" t="n">
-        <v>0.7729563626298884</v>
+        <v>7.54789504187429</v>
       </c>
       <c r="M298" t="n">
         <v>1.292377926583012</v>
@@ -17479,7 +17479,7 @@
         <v>0.04022809207804631</v>
       </c>
       <c r="L299" t="n">
-        <v>1.174403450842987</v>
+        <v>5.608332602049135</v>
       </c>
       <c r="M299" t="n">
         <v>1.183098648135833</v>
@@ -17536,7 +17536,7 @@
         <v>0.01341476640892952</v>
       </c>
       <c r="L300" t="n">
-        <v>0.4276580986630788</v>
+        <v>12.99180561295121</v>
       </c>
       <c r="M300" t="n">
         <v>1.056871590679215</v>
@@ -17590,10 +17590,10 @@
         <v>0.7197447691915825</v>
       </c>
       <c r="K301" t="n">
-        <v>-0.01767689918646374</v>
+        <v>0.01767689918646374</v>
       </c>
       <c r="L301" t="n">
-        <v>0.5978557513614529</v>
+        <v>10.55045059684277</v>
       </c>
       <c r="M301" t="n">
         <v>1.059674905140378</v>
@@ -17650,7 +17650,7 @@
         <v>0.01044299131157145</v>
       </c>
       <c r="L302" t="n">
-        <v>0.2045266658838914</v>
+        <v>10.11659896408848</v>
       </c>
       <c r="M302" t="n">
         <v>1.039703981839993</v>
@@ -17707,7 +17707,7 @@
         <v>0.009443819247439115</v>
       </c>
       <c r="L303" t="n">
-        <v>0.1827752631136259</v>
+        <v>10.27300234667061</v>
       </c>
       <c r="M303" t="n">
         <v>1.015403509129177</v>
@@ -17764,7 +17764,7 @@
         <v>0.009208771102969157</v>
       </c>
       <c r="L304" t="n">
-        <v>0.1805020008494308</v>
+        <v>10.42020993269425</v>
       </c>
       <c r="M304" t="n">
         <v>1.005459967628836</v>
@@ -17818,10 +17818,10 @@
         <v>0.4483444450876536</v>
       </c>
       <c r="K305" t="n">
-        <v>-0.008939879767943887</v>
+        <v>0.008939879767943887</v>
       </c>
       <c r="L305" t="n">
-        <v>0.1502707981689037</v>
+        <v>9.970562274291794</v>
       </c>
       <c r="M305" t="n">
         <v>1.010752173211257</v>
@@ -17875,10 +17875,10 @@
         <v>0.4646187331201314</v>
       </c>
       <c r="K306" t="n">
-        <v>-0.009204333764841647</v>
+        <v>0.009204333764841647</v>
       </c>
       <c r="L306" t="n">
-        <v>0.1834571802375607</v>
+        <v>10.46774316486645</v>
       </c>
       <c r="M306" t="n">
         <v>1.009946175167969</v>
@@ -17932,10 +17932,10 @@
         <v>0.4826595921211929</v>
       </c>
       <c r="K307" t="n">
-        <v>-0.009656405408923848</v>
+        <v>0.009656405408923848</v>
       </c>
       <c r="L307" t="n">
-        <v>0.188885934195228</v>
+        <v>10.66201943691488</v>
       </c>
       <c r="M307" t="n">
         <v>1.027520143849838</v>
@@ -17989,10 +17989,10 @@
         <v>0.5700001100126803</v>
       </c>
       <c r="K308" t="n">
-        <v>-0.01231180140262677</v>
+        <v>0.01231180140262677</v>
       </c>
       <c r="L308" t="n">
-        <v>0.2384922428933852</v>
+        <v>10.80262355275719</v>
       </c>
       <c r="M308" t="n">
         <v>1.121892886493918</v>
@@ -18046,10 +18046,10 @@
         <v>0.5588292694519187</v>
       </c>
       <c r="K309" t="n">
-        <v>-0.01169153302930799</v>
+        <v>0.01169153302930799</v>
       </c>
       <c r="L309" t="n">
-        <v>0.23036926618943</v>
+        <v>11.28865340580673</v>
       </c>
       <c r="M309" t="n">
         <v>1.112623392142308</v>
@@ -18103,10 +18103,10 @@
         <v>0.6348876658787617</v>
       </c>
       <c r="K310" t="n">
-        <v>-0.01421053653406964</v>
+        <v>0.01421053653406964</v>
       </c>
       <c r="L310" t="n">
-        <v>0.2779715242925409</v>
+        <v>11.20514150899453</v>
       </c>
       <c r="M310" t="n">
         <v>1.183640292947201</v>
@@ -18163,7 +18163,7 @@
         <v>0.01196986783072696</v>
       </c>
       <c r="L311" t="n">
-        <v>0.2318356436106103</v>
+        <v>10.6631595428774</v>
       </c>
       <c r="M311" t="n">
         <v>1.097457725849015</v>
@@ -18217,10 +18217,10 @@
         <v>0.4729050740699995</v>
       </c>
       <c r="K312" t="n">
-        <v>-0.009451513395192681</v>
+        <v>0.009451513395192681</v>
       </c>
       <c r="L312" t="n">
-        <v>0.1703482587150926</v>
+        <v>10.46807534101148</v>
       </c>
       <c r="M312" t="n">
         <v>1.0224831818252</v>
@@ -18277,7 +18277,7 @@
         <v>0.01053654381856876</v>
       </c>
       <c r="L313" t="n">
-        <v>0.1621246866121777</v>
+        <v>9.17208628454236</v>
       </c>
       <c r="M313" t="n">
         <v>1.100064499582804</v>
@@ -18334,7 +18334,7 @@
         <v>0.01069974663569855</v>
       </c>
       <c r="L314" t="n">
-        <v>0.1587606398844408</v>
+        <v>10.1967300611219</v>
       </c>
       <c r="M314" t="n">
         <v>1.166109247372863</v>
@@ -18391,7 +18391,7 @@
         <v>0.01238158657123088</v>
       </c>
       <c r="L315" t="n">
-        <v>0.2013944319916148</v>
+        <v>10.07797792328821</v>
       </c>
       <c r="M315" t="n">
         <v>1.182211013481608</v>
@@ -18445,10 +18445,10 @@
         <v>0.5379350555189197</v>
       </c>
       <c r="K316" t="n">
-        <v>-0.01158460167171707</v>
+        <v>0.01158460167171707</v>
       </c>
       <c r="L316" t="n">
-        <v>0.2168759019472745</v>
+        <v>10.25592782712643</v>
       </c>
       <c r="M316" t="n">
         <v>1.109019378057013</v>
@@ -18502,10 +18502,10 @@
         <v>0.4911096912463142</v>
       </c>
       <c r="K317" t="n">
-        <v>-0.01006984028524602</v>
+        <v>0.01006984028524602</v>
       </c>
       <c r="L317" t="n">
-        <v>0.1931296873168972</v>
+        <v>10.32851714287693</v>
       </c>
       <c r="M317" t="n">
         <v>1.041715426720456</v>
@@ -18562,7 +18562,7 @@
         <v>0.01052053154652624</v>
       </c>
       <c r="L318" t="n">
-        <v>0.2130919970413931</v>
+        <v>10.99695283038553</v>
       </c>
       <c r="M318" t="n">
         <v>1.069732877684676</v>
@@ -18616,10 +18616,10 @@
         <v>0.6489999506630775</v>
       </c>
       <c r="K319" t="n">
-        <v>-0.0145526723472561</v>
+        <v>0.0145526723472561</v>
       </c>
       <c r="L319" t="n">
-        <v>0.2974840379902445</v>
+        <v>11.41290271293819</v>
       </c>
       <c r="M319" t="n">
         <v>1.205535016124333</v>
@@ -18676,7 +18676,7 @@
         <v>0.007171264515582501</v>
       </c>
       <c r="L320" t="n">
-        <v>0.1156309936574483</v>
+        <v>12.89661330944876</v>
       </c>
       <c r="M320" t="n">
         <v>1.037875704464434</v>
@@ -18730,10 +18730,10 @@
         <v>0.4703964660590457</v>
       </c>
       <c r="K321" t="n">
-        <v>-0.00839153403910251</v>
+        <v>0.00839153403910251</v>
       </c>
       <c r="L321" t="n">
-        <v>0.1486718581383515</v>
+        <v>13.06944232261491</v>
       </c>
       <c r="M321" t="n">
         <v>1.086799088095669</v>
@@ -18787,10 +18787,10 @@
         <v>1.690136148229345</v>
       </c>
       <c r="K322" t="n">
-        <v>-0.02980482576386681</v>
+        <v>0.02980482576386681</v>
       </c>
       <c r="L322" t="n">
-        <v>5.572651472331713</v>
+        <v>48.05510418960585</v>
       </c>
       <c r="M322" t="n">
         <v>1.180546755291233</v>
@@ -18844,10 +18844,10 @@
         <v>0.9619472488144172</v>
       </c>
       <c r="K323" t="n">
-        <v>-0.01095992334691918</v>
+        <v>0.01095992334691918</v>
       </c>
       <c r="L323" t="n">
-        <v>1.689326126055657</v>
+        <v>65.52188207036382</v>
       </c>
       <c r="M323" t="n">
         <v>1.001227117158517</v>
@@ -18904,7 +18904,7 @@
         <v>0.01031519012025371</v>
       </c>
       <c r="L324" t="n">
-        <v>1.417034346604719</v>
+        <v>62.03729257251617</v>
       </c>
       <c r="M324" t="n">
         <v>1.001184408610791</v>
@@ -18961,7 +18961,7 @@
         <v>0.02062725119907469</v>
       </c>
       <c r="L325" t="n">
-        <v>5.94232830212904</v>
+        <v>65.90681985205656</v>
       </c>
       <c r="M325" t="n">
         <v>1.00376273681954</v>
@@ -19018,7 +19018,7 @@
         <v>0.04001816300564193</v>
       </c>
       <c r="L326" t="n">
-        <v>7.972250756882341</v>
+        <v>41.53816804130398</v>
       </c>
       <c r="M326" t="n">
         <v>1.215865635858974</v>
@@ -19072,10 +19072,10 @@
         <v>2.400509131581272</v>
       </c>
       <c r="K327" t="n">
-        <v>-0.07096418072644682</v>
+        <v>0.07096418072644682</v>
       </c>
       <c r="L327" t="n">
-        <v>16.74617942908024</v>
+        <v>24.28730502414246</v>
       </c>
       <c r="M327" t="n">
         <v>1.160001205682978</v>
@@ -19129,10 +19129,10 @@
         <v>1.970736236269739</v>
       </c>
       <c r="K328" t="n">
-        <v>-0.05708155452318205</v>
+        <v>0.05708155452318205</v>
       </c>
       <c r="L328" t="n">
-        <v>11.51660104994818</v>
+        <v>20.77024163648144</v>
       </c>
       <c r="M328" t="n">
         <v>1.079765896038497</v>
@@ -19186,10 +19186,10 @@
         <v>1.938094078738179</v>
       </c>
       <c r="K329" t="n">
-        <v>-0.04168815570444282</v>
+        <v>0.04168815570444282</v>
       </c>
       <c r="L329" t="n">
-        <v>13.80096408018417</v>
+        <v>37.03794019934956</v>
       </c>
       <c r="M329" t="n">
         <v>1.002404749650312</v>
@@ -19246,7 +19246,7 @@
         <v>0.03979268250241914</v>
       </c>
       <c r="L330" t="n">
-        <v>11.06123082661159</v>
+        <v>32.67298267744476</v>
       </c>
       <c r="M330" t="n">
         <v>1.003297323367846</v>
@@ -19300,10 +19300,10 @@
         <v>1.548798070073161</v>
       </c>
       <c r="K331" t="n">
-        <v>-0.02967408679388077</v>
+        <v>0.02967408679388077</v>
       </c>
       <c r="L331" t="n">
-        <v>3.900530009512029</v>
+        <v>37.30588075315521</v>
       </c>
       <c r="M331" t="n">
         <v>1.215397419843297</v>
@@ -19357,10 +19357,10 @@
         <v>2.569012101875873</v>
       </c>
       <c r="K332" t="n">
-        <v>-0.06240916861774146</v>
+        <v>0.06240916861774146</v>
       </c>
       <c r="L332" t="n">
-        <v>11.8785522541471</v>
+        <v>38.49012154385603</v>
       </c>
       <c r="M332" t="n">
         <v>1.393532279815318</v>
@@ -19417,7 +19417,7 @@
         <v>0.01928969316760852</v>
       </c>
       <c r="L333" t="n">
-        <v>1.595776076037218</v>
+        <v>25.86604830183173</v>
       </c>
       <c r="M333" t="n">
         <v>1.086767365876032</v>
@@ -19474,7 +19474,7 @@
         <v>0.03089777896466362</v>
       </c>
       <c r="L334" t="n">
-        <v>5.407005046751949</v>
+        <v>48.9373626614715</v>
       </c>
       <c r="M334" t="n">
         <v>1.228400009764799</v>
@@ -19528,10 +19528,10 @@
         <v>2.124812778608998</v>
       </c>
       <c r="K335" t="n">
-        <v>-0.05454246066912172</v>
+        <v>0.05454246066912172</v>
       </c>
       <c r="L335" t="n">
-        <v>9.27500242491017</v>
+        <v>28.5128205571173</v>
       </c>
       <c r="M335" t="n">
         <v>1.249277825711376</v>
@@ -19588,7 +19588,7 @@
         <v>0.02779153497145821</v>
       </c>
       <c r="L336" t="n">
-        <v>7.069767991363892</v>
+        <v>44.76971816069594</v>
       </c>
       <c r="M336" t="n">
         <v>1.002680078659296</v>
@@ -19642,10 +19642,10 @@
         <v>1.014307894738269</v>
       </c>
       <c r="K337" t="n">
-        <v>-0.01338827059020756</v>
+        <v>0.01338827059020756</v>
       </c>
       <c r="L337" t="n">
-        <v>1.6772947694005</v>
+        <v>51.47638984744779</v>
       </c>
       <c r="M337" t="n">
         <v>1.057748424916756</v>
@@ -19702,7 +19702,7 @@
         <v>0.04693431657866213</v>
       </c>
       <c r="L338" t="n">
-        <v>12.15001971205299</v>
+        <v>26.5564009080161</v>
       </c>
       <c r="M338" t="n">
         <v>1.009568546202518</v>
@@ -19759,7 +19759,7 @@
         <v>0.02303624380452628</v>
       </c>
       <c r="L339" t="n">
-        <v>3.667452402476256</v>
+        <v>45.77815651221156</v>
       </c>
       <c r="M339" t="n">
         <v>1.123693340408948</v>
@@ -19816,7 +19816,7 @@
         <v>0.03682290159092313</v>
       </c>
       <c r="L340" t="n">
-        <v>7.561857116059479</v>
+        <v>58.12649209268896</v>
       </c>
       <c r="M340" t="n">
         <v>1.308290068486735</v>
@@ -19870,10 +19870,10 @@
         <v>1.068442806272141</v>
       </c>
       <c r="K341" t="n">
-        <v>-0.01208240599591587</v>
+        <v>0.01208240599591587</v>
       </c>
       <c r="L341" t="n">
-        <v>1.526386235683874</v>
+        <v>73.87451025185891</v>
       </c>
       <c r="M341" t="n">
         <v>1.123304883963692</v>
@@ -19930,7 +19930,7 @@
         <v>0.1010646666228089</v>
       </c>
       <c r="L342" t="n">
-        <v>5.467007917531831</v>
+        <v>3.414733921327196</v>
       </c>
       <c r="M342" t="n">
         <v>1.096663364013115</v>
@@ -19984,10 +19984,10 @@
         <v>1.129913721786471</v>
       </c>
       <c r="K343" t="n">
-        <v>-0.06424020448521869</v>
+        <v>0.06424020448521869</v>
       </c>
       <c r="L343" t="n">
-        <v>2.552483484168709</v>
+        <v>3.090791046734364</v>
       </c>
       <c r="M343" t="n">
         <v>1.025590622251829</v>
@@ -20044,7 +20044,7 @@
         <v>0.07074115815386237</v>
       </c>
       <c r="L344" t="n">
-        <v>3.027642365041072</v>
+        <v>3.307849550477762</v>
       </c>
       <c r="M344" t="n">
         <v>1.056623108537044</v>
@@ -20101,7 +20101,7 @@
         <v>0.1056546020519748</v>
       </c>
       <c r="L345" t="n">
-        <v>5.434458513763184</v>
+        <v>3.283769176246734</v>
       </c>
       <c r="M345" t="n">
         <v>1.1247893217002</v>
@@ -20158,7 +20158,7 @@
         <v>0.06630250946944422</v>
       </c>
       <c r="L346" t="n">
-        <v>2.681472608477108</v>
+        <v>3.189311001492414</v>
       </c>
       <c r="M346" t="n">
         <v>1.040972225944959</v>
@@ -20212,10 +20212,10 @@
         <v>1.278391687896268</v>
       </c>
       <c r="K347" t="n">
-        <v>-0.07349293525584126</v>
+        <v>0.07349293525584126</v>
       </c>
       <c r="L347" t="n">
-        <v>3.290110653592428</v>
+        <v>3.420174422645859</v>
       </c>
       <c r="M347" t="n">
         <v>1.059920596820493</v>
@@ -20272,7 +20272,7 @@
         <v>0.08108421043531604</v>
       </c>
       <c r="L348" t="n">
-        <v>3.768937164446817</v>
+        <v>3.461992933116636</v>
       </c>
       <c r="M348" t="n">
         <v>1.057207736302387</v>
@@ -20326,10 +20326,10 @@
         <v>1.228181158692432</v>
       </c>
       <c r="K349" t="n">
-        <v>-0.07157977889307791</v>
+        <v>0.07157977889307791</v>
       </c>
       <c r="L349" t="n">
-        <v>2.975605767981044</v>
+        <v>3.197085224972845</v>
       </c>
       <c r="M349" t="n">
         <v>1.059174083692428</v>
@@ -20383,10 +20383,10 @@
         <v>1.367255653760093</v>
       </c>
       <c r="K350" t="n">
-        <v>-0.07675117684764124</v>
+        <v>0.07675117684764124</v>
       </c>
       <c r="L350" t="n">
-        <v>3.996113836239196</v>
+        <v>3.836425098403934</v>
       </c>
       <c r="M350" t="n">
         <v>1.05822489588138</v>
@@ -20440,10 +20440,10 @@
         <v>1.340370076979389</v>
       </c>
       <c r="K351" t="n">
-        <v>-0.07486358358521333</v>
+        <v>0.07486358358521333</v>
       </c>
       <c r="L351" t="n">
-        <v>3.896677618549994</v>
+        <v>3.799098675950047</v>
       </c>
       <c r="M351" t="n">
         <v>1.052871653463542</v>
@@ -20497,10 +20497,10 @@
         <v>1.387186959553026</v>
       </c>
       <c r="K352" t="n">
-        <v>-0.0784237410625436</v>
+        <v>0.0784237410625436</v>
       </c>
       <c r="L352" t="n">
-        <v>3.35646991562552</v>
+        <v>3.837580579537211</v>
       </c>
       <c r="M352" t="n">
         <v>1.148605937730701</v>
@@ -20557,7 +20557,7 @@
         <v>0.06614451296972551</v>
       </c>
       <c r="L353" t="n">
-        <v>2.710012972320052</v>
+        <v>3.033599312985072</v>
       </c>
       <c r="M353" t="n">
         <v>1.016861938348322</v>
@@ -20614,7 +20614,7 @@
         <v>0.1068790180234516</v>
       </c>
       <c r="L354" t="n">
-        <v>5.196827015533664</v>
+        <v>3.517730970594719</v>
       </c>
       <c r="M354" t="n">
         <v>1.186109901596592</v>
@@ -20668,10 +20668,10 @@
         <v>1.153980732711154</v>
       </c>
       <c r="K355" t="n">
-        <v>-0.06093584910025166</v>
+        <v>0.06093584910025166</v>
       </c>
       <c r="L355" t="n">
-        <v>2.006802943694379</v>
+        <v>3.659296207244447</v>
       </c>
       <c r="M355" t="n">
         <v>1.110320887900874</v>
@@ -20728,7 +20728,7 @@
         <v>0.06247424937127163</v>
       </c>
       <c r="L356" t="n">
-        <v>2.322280297583482</v>
+        <v>3.346702748256439</v>
       </c>
       <c r="M356" t="n">
         <v>1.065685494729359</v>
@@ -20782,10 +20782,10 @@
         <v>1.759096738969238</v>
       </c>
       <c r="K357" t="n">
-        <v>-0.1123937568693457</v>
+        <v>0.1123937568693457</v>
       </c>
       <c r="L357" t="n">
-        <v>6.727492079311692</v>
+        <v>3.810065314872497</v>
       </c>
       <c r="M357" t="n">
         <v>1.155859406185653</v>
@@ -20839,10 +20839,10 @@
         <v>1.720595766722361</v>
       </c>
       <c r="K358" t="n">
-        <v>-0.1110370106621296</v>
+        <v>0.1110370106621296</v>
       </c>
       <c r="L358" t="n">
-        <v>5.793560941684796</v>
+        <v>3.652991437931606</v>
       </c>
       <c r="M358" t="n">
         <v>1.172151353858028</v>
@@ -20899,7 +20899,7 @@
         <v>0.1061402306182739</v>
       </c>
       <c r="L359" t="n">
-        <v>4.50429037814134</v>
+        <v>3.310820000048265</v>
       </c>
       <c r="M359" t="n">
         <v>1.212074949004053</v>
@@ -20956,7 +20956,7 @@
         <v>0.09717466997443533</v>
       </c>
       <c r="L360" t="n">
-        <v>5.128900923266642</v>
+        <v>3.510269776572704</v>
       </c>
       <c r="M360" t="n">
         <v>1.102349254350227</v>
@@ -21013,7 +21013,7 @@
         <v>0.05841397107543323</v>
       </c>
       <c r="L361" t="n">
-        <v>2.139260072110863</v>
+        <v>3.365208971133878</v>
       </c>
       <c r="M361" t="n">
         <v>1.050451851692239</v>
@@ -21070,7 +21070,7 @@
         <v>0.07031189313314641</v>
       </c>
       <c r="L362" t="n">
-        <v>5.478233743781159</v>
+        <v>5.415833474637139</v>
       </c>
       <c r="M362" t="n">
         <v>1.013010888850717</v>
@@ -21127,7 +21127,7 @@
         <v>0.06533027752047005</v>
       </c>
       <c r="L363" t="n">
-        <v>3.56564278274364</v>
+        <v>4.828923855897886</v>
       </c>
       <c r="M363" t="n">
         <v>1.059469501619622</v>
@@ -21181,10 +21181,10 @@
         <v>0.791923539149786</v>
       </c>
       <c r="K364" t="n">
-        <v>-0.04539836568593103</v>
+        <v>0.04539836568593103</v>
       </c>
       <c r="L364" t="n">
-        <v>0.9432375455500464</v>
+        <v>2.130673700779467</v>
       </c>
       <c r="M364" t="n">
         <v>1.001138552152769</v>
@@ -21241,7 +21241,7 @@
         <v>0.08112173368791467</v>
       </c>
       <c r="L365" t="n">
-        <v>6.897491369792971</v>
+        <v>5.722474226121526</v>
       </c>
       <c r="M365" t="n">
         <v>1.003355328680952</v>
@@ -21298,7 +21298,7 @@
         <v>0.3205851848561749</v>
       </c>
       <c r="L366" t="n">
-        <v>29.31123920162771</v>
+        <v>1.612916489909702</v>
       </c>
       <c r="M366" t="n">
         <v>1.031212255343376</v>
@@ -21355,7 +21355,7 @@
         <v>0.08980180098231136</v>
       </c>
       <c r="L367" t="n">
-        <v>3.917356031009971</v>
+        <v>2.302318959836833</v>
       </c>
       <c r="M367" t="n">
         <v>1.006848233969971</v>
@@ -21412,7 +21412,7 @@
         <v>0.1087805841654382</v>
       </c>
       <c r="L368" t="n">
-        <v>4.089167241293127</v>
+        <v>1.635174092171696</v>
       </c>
       <c r="M368" t="n">
         <v>1.005881921211093</v>
@@ -21469,7 +21469,7 @@
         <v>0.176509196545899</v>
       </c>
       <c r="L369" t="n">
-        <v>8.539375050487072</v>
+        <v>1.512716719459896</v>
       </c>
       <c r="M369" t="n">
         <v>1.060192802205628</v>
@@ -21523,10 +21523,10 @@
         <v>1.717277615377026</v>
       </c>
       <c r="K370" t="n">
-        <v>-0.1534865467918154</v>
+        <v>0.1534865467918154</v>
       </c>
       <c r="L370" t="n">
-        <v>8.527123983742397</v>
+        <v>1.900765422170527</v>
       </c>
       <c r="M370" t="n">
         <v>1.042754371596605</v>
@@ -21583,7 +21583,7 @@
         <v>0.1346872966095357</v>
       </c>
       <c r="L371" t="n">
-        <v>5.813876659261312</v>
+        <v>1.530481105592847</v>
       </c>
       <c r="M371" t="n">
         <v>1.010051836213668</v>
@@ -21637,10 +21637,10 @@
         <v>1.645598099133824</v>
       </c>
       <c r="K372" t="n">
-        <v>-0.1612255811411784</v>
+        <v>0.1612255811411784</v>
       </c>
       <c r="L372" t="n">
-        <v>8.058124660234744</v>
+        <v>1.515831946002533</v>
       </c>
       <c r="M372" t="n">
         <v>1.01789544707505</v>
@@ -21694,10 +21694,10 @@
         <v>1.788074504420433</v>
       </c>
       <c r="K373" t="n">
-        <v>-0.1588073704737064</v>
+        <v>0.1588073704737064</v>
       </c>
       <c r="L373" t="n">
-        <v>6.151342296799917</v>
+        <v>2.004301951209195</v>
       </c>
       <c r="M373" t="n">
         <v>1.186045068902355</v>
@@ -21754,7 +21754,7 @@
         <v>0.07200304801890564</v>
       </c>
       <c r="L374" t="n">
-        <v>2.518248256378973</v>
+        <v>2.289823360418969</v>
       </c>
       <c r="M374" t="n">
         <v>1.004646826905757</v>
@@ -21811,7 +21811,7 @@
         <v>0.05292637792694822</v>
       </c>
       <c r="L375" t="n">
-        <v>1.784203032116703</v>
+        <v>3.061128712265267</v>
       </c>
       <c r="M375" t="n">
         <v>1.012297603204271</v>
@@ -21868,7 +21868,7 @@
         <v>0.05846746087889483</v>
       </c>
       <c r="L376" t="n">
-        <v>1.659465954002783</v>
+        <v>2.716258998774707</v>
       </c>
       <c r="M376" t="n">
         <v>1.065031879102517</v>
@@ -21922,10 +21922,10 @@
         <v>1.551230270606101</v>
       </c>
       <c r="K377" t="n">
-        <v>-0.1108024871349089</v>
+        <v>0.1108024871349089</v>
       </c>
       <c r="L377" t="n">
-        <v>7.024501049280204</v>
+        <v>2.688298077979623</v>
       </c>
       <c r="M377" t="n">
         <v>1.002568008824928</v>
@@ -21979,10 +21979,10 @@
         <v>1.20796240656528</v>
       </c>
       <c r="K378" t="n">
-        <v>-0.08195478126687847</v>
+        <v>0.08195478126687847</v>
       </c>
       <c r="L378" t="n">
-        <v>3.174492817599544</v>
+        <v>2.320380950900943</v>
       </c>
       <c r="M378" t="n">
         <v>1.008405416680219</v>
@@ -22036,10 +22036,10 @@
         <v>1.787406543908675</v>
       </c>
       <c r="K379" t="n">
-        <v>-0.1508242675417311</v>
+        <v>0.1508242675417311</v>
       </c>
       <c r="L379" t="n">
-        <v>6.205034603693893</v>
+        <v>2.219602511530196</v>
       </c>
       <c r="M379" t="n">
         <v>1.183389207106829</v>
@@ -22093,10 +22093,10 @@
         <v>1.282374047237691</v>
       </c>
       <c r="K380" t="n">
-        <v>-0.108103931512717</v>
+        <v>0.108103931512717</v>
       </c>
       <c r="L380" t="n">
-        <v>3.945459767692042</v>
+        <v>1.595544090480215</v>
       </c>
       <c r="M380" t="n">
         <v>1.006400998759861</v>
@@ -22153,7 +22153,7 @@
         <v>0.1043209934438642</v>
       </c>
       <c r="L381" t="n">
-        <v>12.67405469926159</v>
+        <v>5.85478269353059</v>
       </c>
       <c r="M381" t="n">
         <v>1.014411231115487</v>

</xml_diff>